<commit_message>
password 변경 및 ppt 추가
</commit_message>
<xml_diff>
--- a/모니터.xlsx
+++ b/모니터.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -421,10 +421,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="52.8" customWidth="1" min="1" max="1"/>
+    <col width="43.2" customWidth="1" min="1" max="1"/>
     <col width="12" customWidth="1" min="2" max="2"/>
     <col width="9.6" customWidth="1" min="3" max="3"/>
-    <col width="1014" customWidth="1" min="4" max="4"/>
+    <col width="1004.4" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -457,7 +457,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>467,730원</t>
+          <t>467,000원</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -467,7 +467,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>https://cr.shopping.naver.com/adcr.nhn?x=OhKSzHmRH0AmH0Aap0yZKv%2F%2F%2Fw%3D%3Ds%2FWZaM8yUCx0QBjF2FkZBh%2BmvugTZcWPC7%2BRYmsvGdkr6D9Doef8fQXU6eDjUh3hFiZQl05vgjID55BiBY6ou7o4WQBe%2FZFkvs1gZ836hbpCe2umHfF2aLgG%2F437Vl%2B2i%2Br%2FdgAtqVYj6DoA7Mm4WZMv%2BjB2erv%2BZ%2Brrs5VHOiTQgGE7%2BZatKjf5hEf1XctkKHHnZ9TKW6MzudMKdsQ1KOpnNrwRClxwG6KI6Xy%2BWtBSkj8Xd80xPWZvn6URexO9BvdrxPgprIfciPgkJT4vsx0Pg%2F6PYJW9LpCSumzPJoigK7CtQzZWLlur1%2FFge4%2BEpoTDxTlVveOAV%2FHtvb1ImQ6MXW5rXgndaI9UHRR4mfeSkudW4LAgR4Xxl%2FdcF1QLK7Z9Jp1LOiLeN5JKqjMaKcN1woZLwre%2F0c6LfC8XQvOYGsxBcpcj%2Bn0m4NCRLi2SBPE5E3LAGtj1RxJnglFPiywqrRpvIAQZSvQnJJtRel5rfVQGkq9cOkjtGo%2BppcJd5wtIYh35n85gCNF9XAudNitgCgu8TH6IETI9IR%2BJIKXdo9SYuXmfGSERDSVFYfuZhS7zg4LGnLNsWxVIJpcUeNAau4fTwOUqyF63FjwpQRls%3D&amp;nvMid=31605413618&amp;catId=50000153</t>
+          <t>https://cr.shopping.naver.com/adcr.nhn?x=w4fD6%2BemTl83JuO%2F9tUOIP%2F%2F%2Fw%3D%3DsqOAUhBvH%2FuKzmkHs%2BtSU7a9mAEF0do95Uf8zdOfs1UpQ3qrx3p0MRIb3ekawSdvJ7xhNl55RfamBMht5a%2Fkc2nfbiCgZda7QnETYwxJl1gGJJ%2Fc0J%2BnoHzQ97jNNHE%2FTaQaOQnHcjvvda2yBa%2BUJJd9%2BKy%2Fm0d%2BgYWHtEf61Jo5CNclKwvLyA%2Fys%2F%2FHPPajL58o0YZDNtixq0MmesgzbxSKH4uGhdMZI%2BTAm7Oh3XZYWq6062OEPPa9WB%2BtWbtCGjgKe6djeuWuGZllC7f3Jz6sJF1TG8DXvuOXRWh2aiSE1QmeK3ZPITzKHcbEnR%2BI8Zi8DMMHaJJ6VXUmUoMOHR965vGBfnBv3%2B4s%2Fk2SNcP5XfqiCwBtPYYwEdSt6i2JAgOJS6a%2BTzf29epXnBQ4gG1UPlbztWGh5QtPCe872fU8Ytq2ME1Xm1HVm1yx1p5EzzNwWY%2BdsNBOvT%2FYv35yUpLuyhUYb3VXENZjLt59b%2BWADdDvNeteddEId2DxjyPLXPNRouOLVBR9bkVCm5wEj0Hs3T4qzSBIVN2HAysFdoOR14Ry0vRE87cjo2dWkxNKhJ%2F%2F%2BQskA5AV77IgvR8e%2FD4KoDr6us%2BRKRCOTdsWr9TI%3D&amp;nvMid=31605413618&amp;catId=50000153</t>
         </is>
       </c>
     </row>
@@ -479,7 +479,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>299,520원</t>
+          <t>299,490원</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -489,7 +489,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>https://cr.shopping.naver.com/adcr.nhn?x=O%2Bdjiq8hiv690sdlxzX7wv%2F%2F%2Fw%3D%3DsMTp%2FcipGj8LB1MDQrlCMAf3UH9%2BSmVvaUOyf52BS59rkEFD9EqEzeuo8lvy6Zeyvz%2Bmv63r1kNC%2F3s8AlKCwPVUDpZsgzFAFORfT0UtaVWZ7h4YxfqVFkPRVarjF1EJTLI7AZ9LZDmHnAQwsi59Cc1Vd6Z%2BmZ5fvTALbBBPmfKJ6LYABWm6lRkxVNeHofoG1CHp%2F7JV%2FSDbR16EgB22aTikbYBqhSVo%2BVMrTfeSHmNZ0UYwtLvFUZlvWLdyGP2oVcBtQ3uJLcsd%2BBJyrtZXBtcOmY27ZGze0Q%2BtXRlM4OxtarJoVrbEtunAYIkKGowOqYc%2F0mRmRwJnZodZv%2BPitSyEhb%2B5%2BbgCLWD5ufmjwVaBxgrKyGzgTjgvZMIoXgNJhxRj%2FAi3dy9FeU1O96ucEQKAhfbmRc6T9Q91MqoVII6p2yfQ3iTSq3wXYkvr6X8dqyAE8ibHq4XStnlPwYvjTJ74VQ0yF3tY7lFQmVbkVWRQ%2BAx%2Bdr38XKVfxUWh2ORwdAYTYOqTv%2FsOm0kcFv3bjpC%2B1Cb%2BupDDRakNJXpW30Qj9CFRyQouNPiiSjBJr1JVSA35CyMrpXQUt3%2FJvHupy5s1ITc7NlRPvorKrNyQBKaY%3D&amp;nvMid=31799047618&amp;catId=50000153</t>
+          <t>https://cr.shopping.naver.com/adcr.nhn?x=9NfJ4Azpu4obVS%2FxYed9of%2F%2F%2Fw%3D%3DsIBDiOwhB%2Fv1fnbwNAD8lTbN8O%2BlhLZSgopR77JWaEJn6D9Doef8fQXU6eDjUh3hFgSqjFD%2FbsFEUlzxbcPT7Lt90lYqjsgb%2Flwx642gSpssQKb3gny%2BhmcHehTHkI9Y9gm95oC2yEe6xrBnXD61GF8v%2BjB2erv%2BZ%2Brrs5VHOiTQgGE7%2BZatKjf5hEf1XctkKtk38bKcbK5fV0XxEiBMVQpnNrwRClxwG6KI6Xy%2BWtBSkj8Xd80xPWZvn6URexO9BvdrxPgprIfciPgkJT4vsx0Pg%2F6PYJW9LpCSumzPJoigK7CtQzZWLlur1%2FFge4%2BEpmT4CJO9WfgP6clOkoKfXA4PEcoRF6RWUsuziSDpD3EykudW4LAgR4Xxl%2FdcF1QLKFzg1DkTmUVo5WUPnPN3YU91woZLwre%2F0c6LfC8XQvOYs6l2z9HXnhuzKc6O1zkYm%2FqF%2Fq%2FJ17EDXjs262KkJxQqrRpvIAQZSvQnJJtRel5pxFiui8cElgR2Eu%2B9nMG1BwtIYh35n85gCNF9XAudNig5m4WdZmdlgz9fvGW92M1bBk5dL6WQn69cSYnrhUc4dS7zg4LGnLNsWxVIJpcUeNAau4fTwOUqyF63FjwpQRls%3D&amp;nvMid=31799047618&amp;catId=50000153</t>
         </is>
       </c>
     </row>
@@ -501,7 +501,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>345,370원</t>
+          <t>345,340원</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -511,7 +511,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>https://cr.shopping.naver.com/adcr.nhn?x=hHa9C2FE0VUA%2BQs3AYT4q%2F%2F%2F%2Fw%3D%3DsDNfwR1nn7LUXczgFXfBXFSJ42r82cq5B6uAa4OcmDK7kEFD9EqEzeuo8lvy6ZeyvQtLvaKKLnZCwbeo%2FJD7Ax1UDpZsgzFAFORfT0UtaVWZ7h4YxfqVFkPRVarjF1EJTLI7AZ9LZDmHnAQwsi59Cc1Vd6Z%2BmZ5fvTALbBBPmfKL%2BHMhXfuiFC4uELuwCB7ZjoiNM5dT4Vt7evHPiFJtimSkbYBqhSVo%2BVMrTfeSHmNZ0UYwtLvFUZlvWLdyGP2oVcBtQ3uJLcsd%2BBJyrtZXBtcOmY27ZGze0Q%2BtXRlM4OxtarJoVrbEtunAYIkKGowOqBcpla%2B8S94P%2B91%2FJO4SD4yEhb%2B5%2BbgCLWD5ufmjwVaBxgrKyGzgTjgvZMIoXgNJhpW3lS%2BqtHc6wKr5SvM7KbKAhfbmRc6T9Q91MqoVII6pHGLOR6DqDGoR%2BSwjkztUno64ifB9DVeZ8ffla9GlFdr7WCezgRTDYvmF1iAiGpPEAwSJT%2BEbJT9CgMdUnENOYYnHIcETcJifOE8sb44IMxQTHTO70tjZ0xLTBj6cW0MN%2B9p7gBNzKzWdXJoRwYsZmxyAhEKTy%2B0Zvtn8oYxIR0Q%3D%3D&amp;nvMid=23692201495&amp;catId=50000153</t>
+          <t>https://cr.shopping.naver.com/adcr.nhn?x=z3Gqhmk3A8Bi1n4vMeFigf%2F%2F%2Fw%3D%3Dstvtlvg3XNun7Z96rlQVXyNFroiCu7v59%2Bsmr%2F5HT6n9Q3qrx3p0MRIb3ekawSdvJoyoy5I4fqTuenULO6q97tXfbiCgZda7QnETYwxJl1gGJJ%2Fc0J%2BnoHzQ97jNNHE%2FTaQaOQnHcjvvda2yBa%2BUJJd9%2BKy%2Fm0d%2BgYWHtEf61Jo5CNclKwvLyA%2Fys%2F%2FHPPajLvWRU0%2FSf5flL335cSfN%2B9SKH4uGhdMZI%2BTAm7Oh3XZYWq6062OEPPa9WB%2BtWbtCGjgKe6djeuWuGZllC7f3Jz6sJF1TG8DXvuOXRWh2aiSE1QmeK3ZPITzKHcbEnR%2BI8SlZVvn71Me77LLfAFjMAtBOQDOcMdyz1KB0KJaXV0QdXfqiCwBtPYYwEdSt6i2JADhk8ZwiEAkDk78SkZ4FfP3FLnmPP1THvRsE06nXbDGjId7fd%2Bwn%2FgkXeEKCjn4sGBkd0uS5719GOL8zcWHfEglJmyxRF5dx5FwNdGXCFbfLtksW9eXyD6JK8nopIYyF1T%2BDzDxwp7nT02YxkVA94lNuwP8vVnM%2BxFO9j8%2BhBBj0toUbT1Skiya%2BssnXWFSKd11SkXvPxCFL9O%2FobcETkVA1QmAmnoJRdq4K9btjkCM0%3D&amp;nvMid=23692201495&amp;catId=50000153</t>
         </is>
       </c>
     </row>
@@ -533,7 +533,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>https://cr.shopping.naver.com/adcr.nhn?x=udks2NvqJ3k4l98YAD6iQ%2F%2F%2F%2Fw%3D%3DscPMJm9Me%2F429AMcpFtQ%2Fv2r4hjra6HBLEEgaZx11J6%2F6D9Doef8fQXU6eDjUh3hF8nAfIzNG0GP9vKXbefLgno4WQBe%2FZFkvs1gZ836hbpCe2umHfF2aLgG%2F437Vl%2B2i%2Br%2FdgAtqVYj6DoA7Mm4WZMv%2BjB2erv%2BZ%2Brrs5VHOiTQgGE7%2BZatKjf5hEf1XctkKEFEeHRefU7bsJqIxa3DxA5nNrwRClxwG6KI6Xy%2BWtBSkj8Xd80xPWZvn6URexO9BvdrxPgprIfciPgkJT4vsx0Pg%2F6PYJW9LpCSumzPJoigK7CtQzZWLlur1%2FFge4%2BEpu%2FZIQGdSuU4gxgqyWDS9LEX2QfW8cdE4IInPWn0YIUSkudW4LAgR4Xxl%2FdcF1QLKOA34JStmBE95WWHkTDxkm24Jfup8rDe4spUk8vsQQKH4HkeWxvxxOV29AgK9CgJ1rBMsrXK4qfOfpEhhbPH8M66oaOaHzfUs1T7KCe3I65%2BwYZCoPBa8DhWD2rbOLHjfnUpTzmQTeleeE0y%2Brv8xbFPUiBnAMS%2Bn3C5nr32eMjtyaCs1eQiShRh1xgxCONzAVoWd0jB03C5aYq3HUc1IKtSSLJQZncWk8e8Ttfjz6Fs%3D&amp;nvMid=23996451524&amp;catId=50000153</t>
+          <t>https://cr.shopping.naver.com/adcr.nhn?x=pARQWx0SVa3JaeJWF2BAYf%2F%2F%2Fw%3D%3Ds36A7MQ2AcO%2BkLv8sA76JQAii1qDqvaSPO3TBs817fj1Q3qrx3p0MRIb3ekawSdvJuIwvZ3XyzwlnlqOn1J9g%2BXfbiCgZda7QnETYwxJl1gGJJ%2Fc0J%2BnoHzQ97jNNHE%2FTaQaOQnHcjvvda2yBa%2BUJJd9%2BKy%2Fm0d%2BgYWHtEf61Jo5CNclKwvLyA%2Fys%2F%2FHPPajLqfFDA8ex50vpt6398tv7KSKH4uGhdMZI%2BTAm7Oh3XZYWq6062OEPPa9WB%2BtWbtCGjgKe6djeuWuGZllC7f3Jz6sJF1TG8DXvuOXRWh2aiSE1QmeK3ZPITzKHcbEnR%2BI8qPeeicgwAJH1NIzwuZnug9pyxX4yGa6B3PMLdJblZfxXfqiCwBtPYYwEdSt6i2JA8Qal2c6PkN2fyQ4qTRePNKWM%2Bwbj8BHdejTYrmahRa7afEZzzDOr%2BEynYnAZf7jivmu2R3xov%2FJITcqnMgyCkltdUqkkP9oySfl7DdkMRyJxTNN%2FHW4dtAy3%2BXx9dZliT%2BDzDxwp7nT02YxkVA94lMCuSL77lwUMgQ2TiviECLcv9s8VlDJIkbOvl2jc6vIDY7RBJx2aPv1bgiR77Jh46w1QmAmnoJRdq4K9btjkCM0%3D&amp;nvMid=23996451524&amp;catId=50000153</t>
         </is>
       </c>
     </row>
@@ -545,7 +545,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>627,100원</t>
+          <t>625,140원</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -555,7 +555,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>https://cr.shopping.naver.com/adcr.nhn?x=v67VGfzu6ziFbSh8z%2BRfNf%2F%2F%2Fw%3D%3DszEfV2XCR%2BdPBsnGiWXRBVc4L8UQnEJGBtP6810Mm9UBQ3qrx3p0MRIb3ekawSdvJiEulGitZJxyt596Fde2i9DF58jfAIBSb%2BHVg6fYTWJTOBrkH5eL%2BGiYgkRcbqqAc3bHOcygeCu4ZWtd%2FrJCted9%2BKy%2Fm0d%2BgYWHtEf61Jo5CNclKwvLyA%2Fys%2F%2FHPPajLQH3hhLE8iHvDmK%2FWAR%2BfXCKH4uGhdMZI%2BTAm7Oh3XZYWq6062OEPPa9WB%2BtWbtCGjgKe6djeuWuGZllC7f3Jz6sJF1TG8DXvuOXRWh2aiSE1QmeK3ZPITzKHcbEnR%2BI8ey4Sh95X2zO2pKV6LfoAMOZKo4gDR6fHdjyrok%2BxlURXfqiCwBtPYYwEdSt6i2JAMShoI5yXi%2BOtCPIRh3O2gbJhEk5Bo6FawgHEnhsGtpQYtq2ME1Xm1HVm1yx1p5Ez247%2FjVnG1Q0J5WXKzp6k8ruyhUYb3VXENZjLt59b%2BWCOMXJ3e9mqDmjTorNkNWkWuTwNPoJbfMpIZmSG%2BZn9TQEiGySRycbLX5VJ9d%2BE5JCschm74tMQloA17xq%2FHSLV4Hd2b%2BreWWld3xl3Q6%2B30UHQIiXcF4qwUXZ2sX76wW8%3D&amp;nvMid=38526777618&amp;catId=50000153</t>
+          <t>https://cr.shopping.naver.com/adcr.nhn?x=M5nyVN1Ejxg8XIdMP4Q0tv%2F%2F%2Fw%3D%3DszpTRspHlE8LlHQ0o8EotGvmF2lqK1fb3quMzk%2FZdl6j6D9Doef8fQXU6eDjUh3hF6yy1Bw0Dr34eJeipu3LSbd90lYqjsgb%2Flwx642gSpssQKb3gny%2BhmcHehTHkI9Y9gm95oC2yEe6xrBnXD61GF8v%2BjB2erv%2BZ%2Brrs5VHOiTQgGE7%2BZatKjf5hEf1XctkKDva%2FZyOdH%2BWjclj6NLMZ%2B5nNrwRClxwG6KI6Xy%2BWtBSkj8Xd80xPWZvn6URexO9BvdrxPgprIfciPgkJT4vsx0Pg%2F6PYJW9LpCSumzPJoigK7CtQzZWLlur1%2FFge4%2BEpSINsHBVJDckAgDOxnQMCKezJ5f7eZ4IZp6QsZ%2F2kPAykudW4LAgR4Xxl%2FdcF1QLKyeMLCuh16%2B3kxvlGzl2btN1woZLwre%2F0c6LfC8XQvOYGsxBcpcj%2Bn0m4NCRLi2SBfMpOkMZ50yGHoRXq6spqFaqnZHSavjXd%2FyVpg0mQgQyXk01CquQAx3RpgBd4tjkxwtIYh35n85gCNF9XAudNih2Ev33u%2BSM2oPZbZjDMxv%2Bgw0L2ai1lpkP8cg%2B4IvHNb1NmOoRBMBsXNQGXzjfbC%2BFUQB%2FrDAzm2q1KHRsHkfE%3D&amp;nvMid=38526777618&amp;catId=50000153</t>
         </is>
       </c>
     </row>
@@ -577,7 +577,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>https://cr.shopping.naver.com/adcr.nhn?x=zv80MWgGaNJoCnIdeBaYKP%2F%2F%2Fw%3D%3DsC9agARlVRVSDtFz2WjT8lgbTNC5xVbLvtEmNdxVW2O3kEFD9EqEzeuo8lvy6ZeyvdSo%2BWFtjjyXQjEn0dt7coFUDpZsgzFAFORfT0UtaVWZ7h4YxfqVFkPRVarjF1EJTLI7AZ9LZDmHnAQwsi59Cc1Vd6Z%2BmZ5fvTALbBBPmfKJ0hbIiXFqcs%2FKOmiYsarS88MnyZ4nyBdKagIazOJHUPykbYBqhSVo%2BVMrTfeSHmNZ0UYwtLvFUZlvWLdyGP2oVcBtQ3uJLcsd%2BBJyrtZXBtcOmY27ZGze0Q%2BtXRlM4OxtarJoVrbEtunAYIkKGowOqYuoVYFaCya49zWJPWkrfvCEhb%2B5%2BbgCLWD5ufmjwVaBxgrKyGzgTjgvZMIoXgNJhCA9VL1NhxgsvyO117WVrvKAhfbmRc6T9Q91MqoVII6qytrQgl%2BNyifFsWLYRKSeCs7CVFcVMP%2FpSxGontpoQfJZMPL1PVSYFyIKUeQ8DdqE4l8gVewsVXFIkbJz2BbVzSFJSU%2BVqJw3J7LPJdf9iFy3F0XLYTlKYa%2BtMrDqXgToBhNg6pO%2F%2Bw6bSRwW%2FduOkoOaPw8DGreU834qq9fiJG%2Fl0xQJ0lj0hTVsWj%2FaHagwDfkLIyuldBS3f8m8e6nLmzUhNzs2VE%2B%2Bisqs3JAEppg%3D%3D&amp;nvMid=20189888243&amp;catId=50000153</t>
+          <t>https://cr.shopping.naver.com/adcr.nhn?x=Tm%2FfJrJuzgeUD5fgQ5qz8f%2F%2F%2Fw%3D%3Dshl7%2F79E0mhSWAyAA8gUsGdjETl%2FO4Eu0A90pHDj4Rt%2F6D9Doef8fQXU6eDjUh3hFYZJ0gPLqbSiTbfyJ%2BVj6D990lYqjsgb%2Flwx642gSpssQKb3gny%2BhmcHehTHkI9Y9gm95oC2yEe6xrBnXD61GF8v%2BjB2erv%2BZ%2Brrs5VHOiTQgGE7%2BZatKjf5hEf1XctkKyUFXXLw6GPVn6AINHWUXrpnNrwRClxwG6KI6Xy%2BWtBSkj8Xd80xPWZvn6URexO9BvdrxPgprIfciPgkJT4vsx0Pg%2F6PYJW9LpCSumzPJoigK7CtQzZWLlur1%2FFge4%2BEp5haJgub4HJOF2kuCn8sJpb6tiOPWuWMQDG9OLlu9axukudW4LAgR4Xxl%2FdcF1QLKYxmHMG%2F9gbs%2BwbUjfQPFhz6FURihOvVNK6%2BarovFEXbHnLkDDphWreS39QoFw9T0Gs6mq772NmusrXvwQlUl2ES2lrliKAhQR9ZAB%2FVBR49Er6RUNc%2F5Yi2PN9QgAp8vPanL2KCSHbzU8480YPWBAsUbe%2F95zAhA9oeUT8%2BfITfC0hiHfmfzmAI0X1cC502KfttFD8%2BaROpnqnqy1yQmHBO2odf2y%2BuWedYGzNf%2FGPqz8ma3SiRL%2FyfwQvpzEN30Bq7h9PA5SrIXrcWPClBGWw%3D%3D&amp;nvMid=20189888243&amp;catId=50000153</t>
         </is>
       </c>
     </row>
@@ -599,7 +599,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>https://cr.shopping.naver.com/adcr.nhn?x=IkioFrxvmU80jbOBCUlXTf%2F%2F%2Fw%3D%3DsxCEOiFuSEMr9X35bjy6c2Nq9fTi2NI1G5rcfgTTQSUv6D9Doef8fQXU6eDjUh3hFWvxpys1DzrLnUA45eR61744WQBe%2FZFkvs1gZ836hbpCe2umHfF2aLgG%2F437Vl%2B2i%2Br%2FdgAtqVYj6DoA7Mm4WZMv%2BjB2erv%2BZ%2Brrs5VHOiTQgGE7%2BZatKjf5hEf1XctkKpT4RCWxZ%2FXR3qXgWc9%2Fvr5nNrwRClxwG6KI6Xy%2BWtBSkj8Xd80xPWZvn6URexO9BvdrxPgprIfciPgkJT4vsx0Pg%2F6PYJW9LpCSumzPJoigK7CtQzZWLlur1%2FFge4%2BEpRGRDXuwbDy02xNfFSrwl2F1f49eVPm8lEyN2MOIBbjKkudW4LAgR4Xxl%2FdcF1QLK15SkdSAjpi9XOyuKZ4w0qbL%2BD79JFqXUHChswIKAa5d9XX8Zqnh%2B%2BuV9YDkvuTYqDVE2OuS%2FxzerRyuvl90vcruyhUYb3VXENZjLt59b%2BWAA8Cg9y1F3L2YZhxXo7bcM7ApIQBoTU1cqRI%2B0ETFqeWbA61eFotY3BN9DaNL7K3y4bkMUxZoGlhL8gddcqk%2FoL9cuZLmaH8AoEmuiYJyFJx0cjwVm1BUYVknE7IEMpz4%3D&amp;nvMid=25744041522&amp;catId=50000153</t>
+          <t>https://cr.shopping.naver.com/adcr.nhn?x=k9QMxLvNM4lP6BWmGzUFC%2F%2F%2F%2Fw%3D%3DsxP2P%2Fgb9wvibeYiKf5r%2Bftq9fTi2NI1G5rcfgTTQSUv6D9Doef8fQXU6eDjUh3hFnCl%2BHqOY3PnoiYFXhK8T0t90lYqjsgb%2Flwx642gSpssQKb3gny%2BhmcHehTHkI9Y9gm95oC2yEe6xrBnXD61GF8v%2BjB2erv%2BZ%2Brrs5VHOiTQgGE7%2BZatKjf5hEf1XctkKpT4RCWxZ%2FXR3qXgWc9%2Fvr5nNrwRClxwG6KI6Xy%2BWtBSkj8Xd80xPWZvn6URexO9BvdrxPgprIfciPgkJT4vsx0Pg%2F6PYJW9LpCSumzPJoigK7CtQzZWLlur1%2FFge4%2BEpVHeB%2FSlTEJy1EowytHVwuSqH05YCd%2BAfZjFut6SbbvGkudW4LAgR4Xxl%2FdcF1QLK15SkdSAjpi9XOyuKZ4w0qbL%2BD79JFqXUHChswIKAa5d9XX8Zqnh%2B%2BuV9YDkvuTYqDVE2OuS%2FxzerRyuvl90vcruyhUYb3VXENZjLt59b%2BWAA8Cg9y1F3L2YZhxXo7bcM7ApIQBoTU1cqRI%2B0ETFqeWbA61eFotY3BN9DaNL7K3y4bkMUxZoGlhL8gddcqk%2FoL9cuZLmaH8AoEmuiYJyFJx0cjwVm1BUYVknE7IEMpz4%3D&amp;nvMid=25744041522&amp;catId=50000153</t>
         </is>
       </c>
     </row>
@@ -621,7 +621,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>https://cr.shopping.naver.com/adcr.nhn?x=yFzCxAiZxgN2qqCeLFCOm%2F%2F%2F%2Fw%3D%3DsZbBKnAm%2BN9NafGgyKnbvduvMAs8cvNfYGlE0Fcho1pz6D9Doef8fQXU6eDjUh3hFzr6nWXeuKwpBHpwP7Rj3aY4WQBe%2FZFkvs1gZ836hbpCe2umHfF2aLgG%2F437Vl%2B2i%2Br%2FdgAtqVYj6DoA7Mm4WZMv%2BjB2erv%2BZ%2Brrs5VHOiTQgGE7%2BZatKjf5hEf1XctkK61XIXqeKfMtJYtpSwzOf8ZnNrwRClxwG6KI6Xy%2BWtBSkj8Xd80xPWZvn6URexO9BvdrxPgprIfciPgkJT4vsx0Pg%2F6PYJW9LpCSumzPJoigK7CtQzZWLlur1%2FFge4%2BEpMBjS5%2FdKFosZhOkEkWJClpO%2FZHfw8y5T72RkNuXQ832kudW4LAgR4Xxl%2FdcF1QLKKeOuYZt6bIyJlMtcMfz5ccb9fe38o2Eslxa66FmBFHbWnL3m3JxqtLHg%2B1iaGH4E%2FMSEQxehWGZnXBvKe4ZUa3IEOMyyDocZ9XLqN14mUSyjriJ8H0NV5nx9%2BVr0aUV2E%2Bos34kDJG9pMGy%2F00iX6SJjEVOA2sbTtnr1tibcKhZicchwRNwmJ84TyxvjggzFL5Us7ROk9u8jRhd1I5Dx8XvdwjKGJ0SkNthNzBkNBJnHICEQpPL7Rm%2B2fyhjEhHR&amp;nvMid=18797620615&amp;catId=50000153</t>
+          <t>https://cr.shopping.naver.com/adcr.nhn?x=WEpsve4pa3SkEYjbj%2F5RXP%2F%2F%2Fw%3D%3DsbwVs9SWuEUE98HG7IHH0N496P0oLvMscg6i%2BtWBO2PPkEFD9EqEzeuo8lvy6Zeyvw7tlmpmGG4itXmlBT1J1Kw2CWj34psFuHU6FoG79mLHoxqQvhEGfzIuiGTUnSeUQIxXmfNKpE7CUL7F3u6%2B2DlVd6Z%2BmZ5fvTALbBBPmfKKCbaAFVOfhA3Yy9Pva8Vi%2FOQ4w%2BfZ1bcQlxT%2BRBP1PyikbYBqhSVo%2BVMrTfeSHmNZ0UYwtLvFUZlvWLdyGP2oVcBtQ3uJLcsd%2BBJyrtZXBtcOmY27ZGze0Q%2BtXRlM4OxtarJoVrbEtunAYIkKGowOq0ar%2Be%2Bhw1xfX242FLCOqFyEhb%2B5%2BbgCLWD5ufmjwVaBxgrKyGzgTjgvZMIoXgNJhxqetWjrEglGkINkekuHdp6AhfbmRc6T9Q91MqoVII6ocMg6Q%2BtcdRun7WGOXd9rxJKh4lz7GIi0OUdfe95lFFMqYMTerNgIP9CYlqfw07NNcZ8pgTGru4bgUYhRhw82x555UuIbm3CB2ihLTi%2B66jiA%2FxrBM0DSpBhXSBSud%2FC6Ov%2B%2BG7P8zZs54SDuTec41064sSc3AnYHDZ2vTmSgHieCgb%2FyEsEDA%2F19u4jxigDbLVWGr8fvvH1mWvUgXPK6j&amp;nvMid=18797620615&amp;catId=50000153</t>
         </is>
       </c>
     </row>
@@ -643,7 +643,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>https://cr.shopping.naver.com/adcr.nhn?x=ECRd%2BNTys2RcBjMyWiYrpP%2F%2F%2Fw%3D%3Ds9hYLXIjqs3NxRUNnck%2Fye%2FNcfCh3lwE1dM9WF95CZet1oC4lxt%2BlhTQccfsXvqj1Xg6L4geA2UhokpnazGUmYQZ8YwQ6cSx0SnSGrjW%2FBwdRV2q10bvim7oXrhLUtXvPHinNrx5sg4hc%2Bs%2BwYZL3l6Tq%2FbD2MGowZHhNOyBhpCfd9mmctTagkO4bZHVBZykEADfJ2wL%2FdOLBhgccxyz%2B8%2B1OtnY4MIPSt%2Bnpndu%2FZgA0fE8zS3oIfwqU6zRcz3TmsWnPZlyLWfVVVeJNqsGWyj9rXyqENDUD8omnd%2BAEOivf3Vb8LXDlJWzaxi1N0VJ6AGGIfRliKSrBTYYO8o5rajokh7KNEkkbwBBKOUFOEEp%2FxPZ%2FIQy%2Bn0YHnsoO5AE1U4djLMls7ZBrQ1QAz2J2SyI28QDIftdPo5sZ73mZF1TsPm2%2B1DF7d5MyxgA9bmDKu7KFRhvdVcQ1mMu3n1v5YHyzuSbYa57YRrkxyciYiPd1EzZ6N5cwcspSFo6AaQgSehkzm6TPp1h0P2FevnkdLzbnppRGbZktR7sG7uB5EcfgtYc14tZJf0mClRt%2B5pN0gqgOvq6z5EpEI5N2xav1Mg%3D%3D&amp;nvMid=24007197522&amp;catId=50000153</t>
+          <t>https://cr.shopping.naver.com/adcr.nhn?x=mNekmLxtHuWDcAt0wkFcTP%2F%2F%2Fw%3D%3DsgB3zS6df2rhofb%2BEZLUB2Nj%2Bc%2B0H887tX9iBl26DI5VQ3qrx3p0MRIb3ekawSdvJqM3Fok%2FYxAlMvUMi%2Bzg77nfbiCgZda7QnETYwxJl1gGJJ%2Fc0J%2BnoHzQ97jNNHE%2FTaQaOQnHcjvvda2yBa%2BUJJd9%2BKy%2Fm0d%2BgYWHtEf61Jo5CNclKwvLyA%2Fys%2F%2FHPPajLCyZd2RJco5u4CakPpKb14yKH4uGhdMZI%2BTAm7Oh3XZYWq6062OEPPa9WB%2BtWbtCGjgKe6djeuWuGZllC7f3Jz6sJF1TG8DXvuOXRWh2aiSE1QmeK3ZPITzKHcbEnR%2BI8P%2Flw%2BLyxUjy%2BpMJlAvHsemHhIPsXBahXQAZk1pvy1OFXfqiCwBtPYYwEdSt6i2JA%2B%2FVTmLSSMxsr18zBLjNWcHf0TZDzrWc0sFfy%2FmfhMFbafEZzzDOr%2BEynYnAZf7jiNU86UGMCVmDikOgluRK%2F9HUeidEoTWPoGQsaBt8KO%2BJRTRTQRqrms63N0Clt9Kl8T%2BDzDxwp7nT02YxkVA94lHgcqZslbqNYNFoj3fS%2BmqpOO1qnF02U1paX2D38HlMVnLywBF6TPdyrHi5pSyQkVg1QmAmnoJRdq4K9btjkCM0%3D&amp;nvMid=24007197522&amp;catId=50000153</t>
         </is>
       </c>
     </row>
@@ -665,7 +665,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>https://cr.shopping.naver.com/adcr.nhn?x=kxgwAocWNnQY%2BOSayhCz5P%2F%2F%2Fw%3D%3Ds2qnM6%2FmWe3L9xcLpALzoXt1XBS1ewTycOeoEOvW8wNj6D9Doef8fQXU6eDjUh3hFDj%2BnE1ve8SC8PZWSMF2Zbo4WQBe%2FZFkvs1gZ836hbpCe2umHfF2aLgG%2F437Vl%2B2i%2Br%2FdgAtqVYj6DoA7Mm4WZMv%2BjB2erv%2BZ%2Brrs5VHOiTQgGE7%2BZatKjf5hEf1XctkKgdH1uPN2p4VrVaA8eoPDfJnNrwRClxwG6KI6Xy%2BWtBSkj8Xd80xPWZvn6URexO9BvdrxPgprIfciPgkJT4vsx0Pg%2F6PYJW9LpCSumzPJoigK7CtQzZWLlur1%2FFge4%2BEpm%2FBpsN60Rfh%2BHr3vg2VSBAkhHjp0TG3RV7NJcgaiVgikudW4LAgR4Xxl%2FdcF1QLK%2F4isSgt%2B5DsqWP8dMcUcoN1woZLwre%2F0c6LfC8XQvOZjBTekaCGYP4998xLPXO53o64ifB9DVeZ8ffla9GlFdhOgNTO4i%2BmwCjyRBw7vcsWenGLqozyA0wl7rU7UadTRYnHIcETcJifOE8sb44IMxdhAwH2UXhl7QPSt2dRVBsEemWcEeWybor1vFYKHLcU9xyAhEKTy%2B0Zvtn8oYxIR0Q%3D%3D&amp;nvMid=35856905618&amp;catId=50000153</t>
+          <t>https://cr.shopping.naver.com/adcr.nhn?x=cck6VHZUotgwMSBftO81Bv%2F%2F%2Fw%3D%3DsXWon8LeskdZ%2BJfJFcUWMZd1XBS1ewTycOeoEOvW8wNj6D9Doef8fQXU6eDjUh3hFu7tZI2UGZ7dkgSaat4wJxd90lYqjsgb%2Flwx642gSpssQKb3gny%2BhmcHehTHkI9Y9gm95oC2yEe6xrBnXD61GF8v%2BjB2erv%2BZ%2Brrs5VHOiTQgGE7%2BZatKjf5hEf1XctkKgdH1uPN2p4VrVaA8eoPDfJnNrwRClxwG6KI6Xy%2BWtBSkj8Xd80xPWZvn6URexO9BvdrxPgprIfciPgkJT4vsx0Pg%2F6PYJW9LpCSumzPJoigK7CtQzZWLlur1%2FFge4%2BEprPUiLxlU3l2kmYgXj3lmcau%2FnOGlfOi%2FjRs2WYmgtW%2BkudW4LAgR4Xxl%2FdcF1QLK%2F4isSgt%2B5DsqWP8dMcUcoN1woZLwre%2F0c6LfC8XQvOZjBTekaCGYP4998xLPXO53o64ifB9DVeZ8ffla9GlFdhOgNTO4i%2BmwCjyRBw7vcsWenGLqozyA0wl7rU7UadTRYnHIcETcJifOE8sb44IMxdhAwH2UXhl7QPSt2dRVBsGhbHQAh1kL7VJj5Qn4kMy6xyAhEKTy%2B0Zvtn8oYxIR0Q%3D%3D&amp;nvMid=35856905618&amp;catId=50000153</t>
         </is>
       </c>
     </row>
@@ -687,7 +687,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>https://cr.shopping.naver.com/adcr.nhn?x=8%2BhuZwzd9JTaPYRc4rlqJv%2F%2F%2Fw%3D%3Ds3Lk6N27W5CGF90xT%2B55k97RB8ySvBnLNeN%2FeCRKqUHvkEFD9EqEzeuo8lvy6ZeyvSK1gZz75SdSjhdtG6I%2FYGlUDpZsgzFAFORfT0UtaVWZ7h4YxfqVFkPRVarjF1EJTLI7AZ9LZDmHnAQwsi59Cc1Vd6Z%2BmZ5fvTALbBBPmfKL392rcVj5mouEkJq8zyckjOvdNzYH3B%2BYyuoul%2BiWoYikbYBqhSVo%2BVMrTfeSHmNZ0UYwtLvFUZlvWLdyGP2oVcBtQ3uJLcsd%2BBJyrtZXBtcOmY27ZGze0Q%2BtXRlM4OxtarJoVrbEtunAYIkKGowOqQ3z27HMQwcD%2Bz5lLzM77OyEhb%2B5%2BbgCLWD5ufmjwVaBxgrKyGzgTjgvZMIoXgNJhim2Hd0yKdWERlWmdMxwfWaAhfbmRc6T9Q91MqoVII6qbwBSvNXx%2FbBIpAXNrvhoFo64ifB9DVeZ8ffla9GlFdpTRFQH63Qz%2F7pdoQlb%2B9Dk1iEq2loxQMveWL1LBkHowYnHIcETcJifOE8sb44IMxXewyHwjkW3ywZ8bnIT9IgH7T5Y8Tr8otDqS6YGkL7wb5Hv1T%2FoDPeAT2ZD%2BWCfnsQ%3D%3D&amp;nvMid=29060355587&amp;catId=50000153</t>
+          <t>https://cr.shopping.naver.com/adcr.nhn?x=fYqhzPZIl%2Foq2q0eg7WnwP%2F%2F%2Fw%3D%3DsHY35apBD6YyumJ6neRvADbstJmSUces3mb5OyhPxOID6D9Doef8fQXU6eDjUh3hFKNiHlpsmch1H5bgJX6j5R990lYqjsgb%2Flwx642gSpssQKb3gny%2BhmcHehTHkI9Y9gm95oC2yEe6xrBnXD61GF8v%2BjB2erv%2BZ%2Brrs5VHOiTQgGE7%2BZatKjf5hEf1XctkK77CMbNkSJqTT3mZeXtMZJpnNrwRClxwG6KI6Xy%2BWtBSkj8Xd80xPWZvn6URexO9BvdrxPgprIfciPgkJT4vsx0Pg%2F6PYJW9LpCSumzPJoigK7CtQzZWLlur1%2FFge4%2BEpVwB9a10Dpa9wTaVoKGjH15jjbpcjIGiC2e%2BSaGbomRGkudW4LAgR4Xxl%2FdcF1QLKA2rQahrHASzOyDV%2B5UfKqXornTeMFMWI76yU7BvGjg4E6sCSFbEeNpleHuJN%2FcsAr%2FX1Ayz5spOceSt0pdK92mYmYWeWvrPdeORBFWgqDDVl7Z%2FLd%2BFWl6O5JW5IFlX6nUpTzmQTeleeE0y%2Brv8xbCPoivkmO0H7r9v6EbH9TzWfoL4BDggSltoBZrbfQz8dA35CyMrpXQUt3%2FJvHupy5s1ITc7NlRPvorKrNyQBKaY%3D&amp;nvMid=29060355587&amp;catId=50000153</t>
         </is>
       </c>
     </row>
@@ -699,7 +699,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>345,130원</t>
+          <t>345,000원</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -709,7 +709,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>https://cr.shopping.naver.com/adcr.nhn?x=OixuoxIggcBj%2FpGNj1s2qv%2F%2F%2Fw%3D%3Ds%2FQZb3HcnGIijRYhZ43ak9Gf4qYIZnYIGua6Z%2BjmAdG%2F6D9Doef8fQXU6eDjUh3hFLXb8FwJokkYJYO7MwqlrpI4WQBe%2FZFkvs1gZ836hbpCe2umHfF2aLgG%2F437Vl%2B2i%2Br%2FdgAtqVYj6DoA7Mm4WZMv%2BjB2erv%2BZ%2Brrs5VHOiTQgGE7%2BZatKjf5hEf1XctkKdtydQAar1N2cU%2FH4PxRk9ZnNrwRClxwG6KI6Xy%2BWtBSkj8Xd80xPWZvn6URexO9BvdrxPgprIfciPgkJT4vsx0Pg%2F6PYJW9LpCSumzPJoigK7CtQzZWLlur1%2FFge4%2BEp5MLsaz8K1qkHCaAi7G0i%2FEtlPt3Efqf4HK1QNaCyl%2BmkudW4LAgR4Xxl%2FdcF1QLKu4afHlRJpaob4mJ3pXDwTdwRQyT5iDRlXdtlKXilPLI3zhGuFQFWE0iDC9qaUVwhi1E1oa2yxk5QufeGHs%2FPIlzchE3UHDOYEqZsCeTpx33I%2Bcrg5e3IsCtUhlISoBYGUTeuJgZvRvEK7gZCw3B0%2Bkvxr4Fk8YIkjUVQGDBnCzgmg7gvaoBXwphjkU7sjPqDPm2V2WLj0oLfvtXSAq9jPg1QmAmnoJRdq4K9btjkCM0%3D&amp;nvMid=32982708620&amp;catId=50000153</t>
+          <t>https://cr.shopping.naver.com/adcr.nhn?x=zaWsOduz1A1wll9i40V%2Faf%2F%2F%2Fw%3D%3DsG2hRZoF5IlRW%2BTYUK1T4YWf4qYIZnYIGua6Z%2BjmAdG%2F6D9Doef8fQXU6eDjUh3hFJsHW%2BRwSIVO2xUhC0doMq990lYqjsgb%2Flwx642gSpssQKb3gny%2BhmcHehTHkI9Y9gm95oC2yEe6xrBnXD61GF8v%2BjB2erv%2BZ%2Brrs5VHOiTQgGE7%2BZatKjf5hEf1XctkKdtydQAar1N2cU%2FH4PxRk9ZnNrwRClxwG6KI6Xy%2BWtBSkj8Xd80xPWZvn6URexO9BvdrxPgprIfciPgkJT4vsx0Pg%2F6PYJW9LpCSumzPJoigK7CtQzZWLlur1%2FFge4%2BEpmv9fQMmDiX8n3wTOgT8JexoMklUWRbwAeKLBtfbMrs2kudW4LAgR4Xxl%2FdcF1QLKu4afHlRJpaob4mJ3pXDwTdwRQyT5iDRlXdtlKXilPLI3zhGuFQFWE0iDC9qaUVwhi1E1oa2yxk5QufeGHs%2FPIlzchE3UHDOYEqZsCeTpx30X4akg%2FJbvtzmOCl3WU6zwUTeuJgZvRvEK7gZCw3B0%2Bkvxr4Fk8YIkjUVQGDBnCzijxbTWsemHRZNetYc0bCw%2BPm2V2WLj0oLfvtXSAq9jPg1QmAmnoJRdq4K9btjkCM0%3D&amp;nvMid=32982708620&amp;catId=50000153</t>
         </is>
       </c>
     </row>
@@ -731,95 +731,95 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>https://cr.shopping.naver.com/adcr.nhn?x=n0Rd9M8zuuiOQmCtWgXzEP%2F%2F%2Fw%3D%3DstOgUQiSr%2FCycvEpuRRqjmHeEvqH7rnLcfv8w8I8lePdQ3qrx3p0MRIb3ekawSdvJ56kInTg38yw39bIAmOQA4zF58jfAIBSb%2BHVg6fYTWJTOBrkH5eL%2BGiYgkRcbqqAc3bHOcygeCu4ZWtd%2FrJCted9%2BKy%2Fm0d%2BgYWHtEf61Jo5CNclKwvLyA%2Fys%2F%2FHPPajLFZMh5zxY7qjqM1kSzrP2%2ByKH4uGhdMZI%2BTAm7Oh3XZYWq6062OEPPa9WB%2BtWbtCGjgKe6djeuWuGZllC7f3Jz6sJF1TG8DXvuOXRWh2aiSE1QmeK3ZPITzKHcbEnR%2BI8KHPll6wSOHmd2vUNTPeKJV0dkNbqTaZtO9994GPAyhtXfqiCwBtPYYwEdSt6i2JA3rZ54u%2FGFShDBCg1von460e4DARkwLZ9kh6rmrEC8Z1VAjJzz%2FoBiR52Md1TqaFVdqCZPYin6rtvNBEKA1IgAT03CHXhJ90DsA8t1KaNamcymBuyNHFXNXd5kXn7%2Bnuw5h5Py00ZP8HSnfNJaBQUe4U4%2FDZtqcGCJ4137bUhVtUZ4RMFYGe3P4ifxFGtqCqQnyUM3Jc7fv629PWmoERYIoKoDr6us%2BRKRCOTdsWr9TI%3D&amp;nvMid=23896119522&amp;catId=50000153</t>
+          <t>https://cr.shopping.naver.com/adcr.nhn?x=SPpvlC%2Bki3o1%2FKtPKKnT4v%2F%2F%2Fw%3D%3Ds8KRBJCKSdAyEXbUygOOnqXeEvqH7rnLcfv8w8I8lePdQ3qrx3p0MRIb3ekawSdvJur%2FbMNzaz7QZDrzDvCXnKHfbiCgZda7QnETYwxJl1gGJJ%2Fc0J%2BnoHzQ97jNNHE%2FTaQaOQnHcjvvda2yBa%2BUJJd9%2BKy%2Fm0d%2BgYWHtEf61Jo5CNclKwvLyA%2Fys%2F%2FHPPajLFZMh5zxY7qjqM1kSzrP2%2ByKH4uGhdMZI%2BTAm7Oh3XZYWq6062OEPPa9WB%2BtWbtCGjgKe6djeuWuGZllC7f3Jz6sJF1TG8DXvuOXRWh2aiSE1QmeK3ZPITzKHcbEnR%2BI8IZvB%2FZ6PZd6LBB6QMgpcXniyebe78yA5UsxjQIS8sSRXfqiCwBtPYYwEdSt6i2JA3rZ54u%2FGFShDBCg1von460e4DARkwLZ9kh6rmrEC8Z1VAjJzz%2FoBiR52Md1TqaFVdqCZPYin6rtvNBEKA1IgAT03CHXhJ90DsA8t1KaNamcymBuyNHFXNXd5kXn7%2Bnuw5h5Py00ZP8HSnfNJaBQUe4U4%2FDZtqcGCJ4137bUhVtUZ4RMFYGe3P4ifxFGtqCqQnyUM3Jc7fv629PWmoERYIoKoDr6us%2BRKRCOTdsWr9TI%3D&amp;nvMid=23896119522&amp;catId=50000153</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>DELL 울트라샤프 U2723QE</t>
+          <t>삼성전자 삼성 S24R350 베젤리스 프리싱크 75</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>489,000원</t>
+          <t>167,894원</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>414개</t>
+          <t>7,871개</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>https://cr.shopping.naver.com/adcr.nhn?x=8eYWHt%2BVPIsyKrkIdgMiXf%2F%2F%2Fw%3D%3Ds5pWtxRZrUjcCzynPvQoCfR9YyKTZ3H5%2FllYlXkTUuNf6D9Doef8fQXU6eDjUh3hFmA03gkEfKv7Npt3%2FSJGFK44WQBe%2FZFkvs1gZ836hbpCe2umHfF2aLgG%2F437Vl%2B2i%2Br%2FdgAtqVYj6DoA7Mm4WZMv%2BjB2erv%2BZ%2Brrs5VHOiTQgGE7%2BZatKjf5hEf1XctkKPJzC1GCBvxFZarQFBgXznJnNrwRClxwG6KI6Xy%2BWtBSkj8Xd80xPWZvn6URexO9BvdrxPgprIfciPgkJT4vsx0Pg%2F6PYJW9LpCSumzPJoigK7CtQzZWLlur1%2FFge4%2BEp5iLJZOqyliYzM3zBexneSktlPt3Efqf4HK1QNaCyl%2BmkudW4LAgR4Xxl%2FdcF1QLKP%2Fic9xrFaIRWqH6EsdTOLkojX3g7fJUZGRMAq7k1lOf2CBSZrZj5gKy2PtXG3Hr15cVQUGIUsFRTZR1A959MqOCugz0KR6msk51XpYkEMNfhbsnGaz2%2F53FYvui1Qgf2nUpTzmQTeleeE0y%2Brv8xbCNW3s5REsop3crk1XxwVXCndKAb2ZmPkyOepP7FWF1OA35CyMrpXQUt3%2FJvHupy5s1ITc7NlRPvorKrNyQBKaY%3D&amp;nvMid=31516928619&amp;catId=50000153</t>
+          <t>https://cr.shopping.naver.com/adcr.nhn?x=k8CFLC2tOwe66j8S8ZYC6P%2F%2F%2Fw%3D%3Dss5VicazSBV0xrxJDEP96LKCcvLIZ2fIvZPgPa2V8rmLkEFD9EqEzeuo8lvy6ZeyvB%2FuGG3iff9qfZ1qcpq9cqg2CWj34psFuHU6FoG79mLHoxqQvhEGfzIuiGTUnSeUQIxXmfNKpE7CUL7F3u6%2B2DlVd6Z%2BmZ5fvTALbBBPmfKJ0hbIiXFqcs%2FKOmiYsarS8jLL%2ButlDWQEQ1yuSrbWVbikbYBqhSVo%2BVMrTfeSHmNZ0UYwtLvFUZlvWLdyGP2oVcBtQ3uJLcsd%2BBJyrtZXBtcOmY27ZGze0Q%2BtXRlM4OxtarJoVrbEtunAYIkKGowOqGdApTPoHNDKHfELzUBMqaSEhb%2B5%2BbgCLWD5ufmjwVaBxgrKyGzgTjgvZMIoXgNJhqwZk5aXKT9rhBS2GlSnOo6AhfbmRc6T9Q91MqoVII6pcjVKq36k0Jy6zOJdE0ExEJxmjRURG9sfByvKK4PRXU1%2F0M3%2FaKKjxo%2BHWV7Bj14dcZ8pgTGru4bgUYhRhw82xqAcBayeMXClYEPZUkfzYES8xEz1CVDr32Oz3s8pc1hGOv%2B%2BG7P8zZs54SDuTec41mkD662hXwgBbN0maK05g0JchzcdBAAIO4hMHIqrtUuLLVWGr8fvvH1mWvUgXPK6j&amp;nvMid=20861526783&amp;catId=50000153</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>삼성전자 삼성 S27C310</t>
+          <t>DELL 울트라샤프 U2723QE</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>187,000원</t>
+          <t>489,000원</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>43개</t>
+          <t>414개</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>https://cr.shopping.naver.com/adcr.nhn?x=sz6SA0g3B%2BPuHMGBtBECIf%2F%2F%2Fw%3D%3Ds9Wuz3G9Wd5ksrsyQPKuEQsL6UVMi5GJwtSOYgJFl6FBQ3qrx3p0MRIb3ekawSdvJtWcEARdu4wNgU28adSD%2FIDF58jfAIBSb%2BHVg6fYTWJTOBrkH5eL%2BGiYgkRcbqqAc3bHOcygeCu4ZWtd%2FrJCted9%2BKy%2Fm0d%2BgYWHtEf61Jo5CNclKwvLyA%2Fys%2F%2FHPPajLi99zZGs5mhkLkTSmGE7oYiKH4uGhdMZI%2BTAm7Oh3XZYWq6062OEPPa9WB%2BtWbtCGjgKe6djeuWuGZllC7f3Jz6sJF1TG8DXvuOXRWh2aiSE1QmeK3ZPITzKHcbEnR%2BI8xn9ILJA3qqvwNYsKWW8GWlWeI%2B4ci5gsCE1Bh1%2F7bc9XfqiCwBtPYYwEdSt6i2JA3YRF0mih8cSj7iqm7jMfXw680anrzfzPbA%2FhSANHim2ITF%2Bn1aaTvXziEq%2F4MxnvwTuDKIcJ%2B%2F83249UD85P41BvIAaonlqWGjb4wlVZ4pRzujugRM%2FI1GyTG%2FB2bBzrT%2BDzDxwp7nT02YxkVA94lPD60rso5%2BGnJ24Ogvoc5sss2TVe59U2OoNeCOm1x%2FeL6Etrp8Nxh8kQ0BVZEWYLrwau4fTwOUqyF63FjwpQRls%3D&amp;nvMid=38607791618&amp;catId=50000153</t>
+          <t>https://cr.shopping.naver.com/adcr.nhn?x=h3muGKBiorq5E8MIWHHDov%2F%2F%2Fw%3D%3Ds6ZBf8OsnnMOTLd7PibKB9B9YyKTZ3H5%2FllYlXkTUuNf6D9Doef8fQXU6eDjUh3hFDWD7aPF8cLkPqqpK4Mu4hN90lYqjsgb%2Flwx642gSpssQKb3gny%2BhmcHehTHkI9Y9gm95oC2yEe6xrBnXD61GF8v%2BjB2erv%2BZ%2Brrs5VHOiTQgGE7%2BZatKjf5hEf1XctkKPJzC1GCBvxFZarQFBgXznJnNrwRClxwG6KI6Xy%2BWtBSkj8Xd80xPWZvn6URexO9BvdrxPgprIfciPgkJT4vsx0Pg%2F6PYJW9LpCSumzPJoigK7CtQzZWLlur1%2FFge4%2BEpBoJRXt4HNjsrspjWlXJifBnark7wkt7WzcXti33PpzKkudW4LAgR4Xxl%2FdcF1QLKP%2Fic9xrFaIRWqH6EsdTOLkojX3g7fJUZGRMAq7k1lOf2CBSZrZj5gKy2PtXG3Hr15cVQUGIUsFRTZR1A959MqOCugz0KR6msk51XpYkEMNfhbsnGaz2%2F53FYvui1Qgf2nUpTzmQTeleeE0y%2Brv8xbPiFysJrE1JwXftXVAuvNz%2BDY3N%2FILErrYKoDJHB62c5A35CyMrpXQUt3%2FJvHupy5s1ITc7NlRPvorKrNyQBKaY%3D&amp;nvMid=31516928619&amp;catId=50000153</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>삼성전자 스마트모니터 M5 S27BM500</t>
+          <t>삼성전자 삼성 S27C310</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>223,730원</t>
+          <t>187,000원</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>566개</t>
+          <t>43개</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>https://cr.shopping.naver.com/adcr.nhn?x=Wco8TOaodcBP1w4kkqQ1bf%2F%2F%2Fw%3D%3DsYMf5VhcNqwav0TJHqxWikRUzcNC5Hw3WF1LZwNiV5JpQ3qrx3p0MRIb3ekawSdvJhsKK2BkbZ3BbjKgnSGC90DF58jfAIBSb%2BHVg6fYTWJTOBrkH5eL%2BGiYgkRcbqqAc3bHOcygeCu4ZWtd%2FrJCted9%2BKy%2Fm0d%2BgYWHtEf61Jo5CNclKwvLyA%2Fys%2F%2FHPPajLJ7ZqSVh0wmoYtDCifSWR3SKH4uGhdMZI%2BTAm7Oh3XZYWq6062OEPPa9WB%2BtWbtCGjgKe6djeuWuGZllC7f3Jz6sJF1TG8DXvuOXRWh2aiSE1QmeK3ZPITzKHcbEnR%2BI8tfnuSf4qu62sBCg%2BobsT3W5sNZQqrzaT0MrP0UGsJwRXfqiCwBtPYYwEdSt6i2JAqu37Lc0m3BkBIsxbim7rD2Qtm4GLbKd8fs8SgBwzfIMYtq2ME1Xm1HVm1yx1p5EzmyaG4CNZGK0Sy%2F2naXMIX7uyhUYb3VXENZjLt59b%2BWBKUBpcdKHq3fD0YMn24%2FzDWnIPsSEV%2FCiyt1j59R3aNns3T4qzSBIVN2HAysFdoORKGxvZXIPmX59qlXmyu43SlmuhK2FQxoyMTlG7qObmeA4SwcLvxUEucVmH%2BcOht40%3D&amp;nvMid=31910890630&amp;catId=50000153</t>
+          <t>https://cr.shopping.naver.com/adcr.nhn?x=tZANSrx%2F930NxKV2YvsfTP%2F%2F%2Fw%3D%3Ds1IkpM%2BlEPDstsq0Jy00dBsL6UVMi5GJwtSOYgJFl6FBQ3qrx3p0MRIb3ekawSdvJbCHpTECZTu8aU7L12Jcx43fbiCgZda7QnETYwxJl1gGJJ%2Fc0J%2BnoHzQ97jNNHE%2FTaQaOQnHcjvvda2yBa%2BUJJd9%2BKy%2Fm0d%2BgYWHtEf61Jo5CNclKwvLyA%2Fys%2F%2FHPPajLi99zZGs5mhkLkTSmGE7oYiKH4uGhdMZI%2BTAm7Oh3XZYWq6062OEPPa9WB%2BtWbtCGjgKe6djeuWuGZllC7f3Jz6sJF1TG8DXvuOXRWh2aiSE1QmeK3ZPITzKHcbEnR%2BI8q88eT8uDoosNVqcyv%2Fu%2BBjaday6QDwVpgpT8iZ9spjdXfqiCwBtPYYwEdSt6i2JA3YRF0mih8cSj7iqm7jMfXw680anrzfzPbA%2FhSANHim2ITF%2Bn1aaTvXziEq%2F4MxnvwTuDKIcJ%2B%2F83249UD85P41BvIAaonlqWGjb4wlVZ4pRzujugRM%2FI1GyTG%2FB2bBzrT%2BDzDxwp7nT02YxkVA94lJRuz3P9teOFm0RfGG5RmeKVfyl7nYNZ%2F3bnQaf1%2F9Ivc7xQNMnx5%2FghfeI4CJpH%2FQau4fTwOUqyF63FjwpQRls%3D&amp;nvMid=38607791618&amp;catId=50000153</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>삼성전자 삼성 S24R350 베젤리스 프리싱크 75</t>
+          <t>삼성전자 스마트모니터 M5 S27BM500</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>167,894원</t>
+          <t>223,730원</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>7,871개</t>
+          <t>566개</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>https://cr.shopping.naver.com/adcr.nhn?x=Bb5OydVgbkhh2LNqvKRRgP%2F%2F%2Fw%3D%3Ds1ctasS%2B2nsK6RQaxsXJU36CcvLIZ2fIvZPgPa2V8rmLkEFD9EqEzeuo8lvy6ZeyvBPqkvNCT0HiO8C%2FJ7Vje%2BlUDpZsgzFAFORfT0UtaVWZ7h4YxfqVFkPRVarjF1EJTLI7AZ9LZDmHnAQwsi59Cc1Vd6Z%2BmZ5fvTALbBBPmfKJ0hbIiXFqcs%2FKOmiYsarS8jLL%2ButlDWQEQ1yuSrbWVbikbYBqhSVo%2BVMrTfeSHmNZ0UYwtLvFUZlvWLdyGP2oVcBtQ3uJLcsd%2BBJyrtZXBtcOmY27ZGze0Q%2BtXRlM4OxtarJoVrbEtunAYIkKGowOqczddXPMxdvdNKxbo2JagICEhb%2B5%2BbgCLWD5ufmjwVaBxgrKyGzgTjgvZMIoXgNJhqwZk5aXKT9rhBS2GlSnOo6AhfbmRc6T9Q91MqoVII6pcjVKq36k0Jy6zOJdE0ExEJxmjRURG9sfByvKK4PRXU1%2F0M3%2FaKKjxo%2BHWV7Bj14dcZ8pgTGru4bgUYhRhw82xqAcBayeMXClYEPZUkfzYES8xEz1CVDr32Oz3s8pc1hGOv%2B%2BG7P8zZs54SDuTec41OtOxjHiaqHxJQ6Q7XKkOhZchzcdBAAIO4hMHIqrtUuLLVWGr8fvvH1mWvUgXPK6j&amp;nvMid=20861526783&amp;catId=50000153</t>
+          <t>https://cr.shopping.naver.com/adcr.nhn?x=2beMZD3yyh38qDUzfL4Wtv%2F%2F%2Fw%3D%3Dsmb6iK%2Fxqten25eiTR94SwQe2TvK8WDFiZuExruYNnsfkEFD9EqEzeuo8lvy6ZeyvxZXuqcPJWs1Kq2eOxz25lQ2CWj34psFuHU6FoG79mLHoxqQvhEGfzIuiGTUnSeUQIxXmfNKpE7CUL7F3u6%2B2DlVd6Z%2BmZ5fvTALbBBPmfKJ6LYABWm6lRkxVNeHofoG1wqvIDHOa0mP9N4lfYTI7ICkbYBqhSVo%2BVMrTfeSHmNZ0UYwtLvFUZlvWLdyGP2oVcBtQ3uJLcsd%2BBJyrtZXBtcOmY27ZGze0Q%2BtXRlM4OxtarJoVrbEtunAYIkKGowOqA1baFOCI%2BUwPTAG8bZ3lSyEhb%2B5%2BbgCLWD5ufmjwVaBxgrKyGzgTjgvZMIoXgNJhDCpj4UuJmFNHljgUFjd%2FvKAhfbmRc6T9Q91MqoVII6rLkmKBce8iyiPdwJc7OJ90yAE8ibHq4XStnlPwYvjTJy9ksTPc5THvj91xdTocIYHvfQA4Lxacaq9ewOJO7jE0AYTYOqTv%2FsOm0kcFv3bjpMQ85Wp7Jh2qTrwdWK8KRfXhTB73bllCRAA5OLQNubCYb1NmOoRBMBsXNQGXzjfbC%2BFUQB%2FrDAzm2q1KHRsHkfE%3D&amp;nvMid=31910890630&amp;catId=50000153</t>
         </is>
       </c>
     </row>
@@ -841,51 +841,51 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>https://cr.shopping.naver.com/adcr.nhn?x=6Q9YwMNksWjCd%2B8PCv55gP%2F%2F%2Fw%3D%3Dsnnl8n6O5Z%2BrrgOX%2BHVu%2B6jnwxDCTccZ1%2BZdC5KPulHz6D9Doef8fQXU6eDjUh3hFhU5HQXtWFe8Mpva6%2BUOi6o4WQBe%2FZFkvs1gZ836hbpCe2umHfF2aLgG%2F437Vl%2B2i%2Br%2FdgAtqVYj6DoA7Mm4WZMv%2BjB2erv%2BZ%2Brrs5VHOiTQgGE7%2BZatKjf5hEf1XctkKPxl3s0MwX6UCDVuI7MaHvJnNrwRClxwG6KI6Xy%2BWtBSkj8Xd80xPWZvn6URexO9BvdrxPgprIfciPgkJT4vsx0Pg%2F6PYJW9LpCSumzPJoigK7CtQzZWLlur1%2FFge4%2BEphXBELjmahpKe2qb8JiHj7UTQe8hljNiyyePLB6gjWsSkudW4LAgR4Xxl%2FdcF1QLK1qxHZq0ZhHBy8BN5tJn6Tz6FURihOvVNK6%2BarovFEXZ9XX8Zqnh%2B%2BuV9YDkvuTYq63UI8YmGLyqsScVZzJuiospayuwgQjFofbn1LTCfj7mxOoMpXEiFX8dC2x%2FUvmr7T%2BDzDxwp7nT02YxkVA94lFyVHNgWlfs6meTBzj4WZ5C1avjjUHzb5xFdt6f00RLshttyjnknnuGMwlaohFRrQAau4fTwOUqyF63FjwpQRls%3D&amp;nvMid=23896004523&amp;catId=50000153</t>
+          <t>https://cr.shopping.naver.com/adcr.nhn?x=3HdvjW3f1oDASNgxkw7Iqv%2F%2F%2Fw%3D%3DsTWFpmRwbXGZaE%2BqW2afI3l%2FfyNd6EUQDn4XBGz9i9tbkEFD9EqEzeuo8lvy6ZeyvmSKld0%2B1dhVgUWs4waFNTA2CWj34psFuHU6FoG79mLHoxqQvhEGfzIuiGTUnSeUQIxXmfNKpE7CUL7F3u6%2B2DlVd6Z%2BmZ5fvTALbBBPmfKL%2BHMhXfuiFC4uELuwCB7ZjMXYkRfyuYyIGWXk%2FeC7sSSkbYBqhSVo%2BVMrTfeSHmNZ0UYwtLvFUZlvWLdyGP2oVcBtQ3uJLcsd%2BBJyrtZXBtcOmY27ZGze0Q%2BtXRlM4OxtarJoVrbEtunAYIkKGowOqbeatkbqu7TdD7jG3gFhXWCEhb%2B5%2BbgCLWD5ufmjwVaBxgrKyGzgTjgvZMIoXgNJhbBi7IS2kuSvVnENTWdmfbaAhfbmRc6T9Q91MqoVII6oOyi2Z1jSN6qPQE0IBo3Nb2wTcnSkbOyfl0nB6iWbIvwObyc1BMert1jIB59NOJVkdqFS7Dqk3z5We7SX%2BRibqnUpTzmQTeleeE0y%2Brv8xbHltjRgtnkiDbXpVCIY28l8xhgR2N%2FehKtxSwNKsLom6A35CyMrpXQUt3%2FJvHupy5s1ITc7NlRPvorKrNyQBKaY%3D&amp;nvMid=23896004523&amp;catId=50000153</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>제우스랩 알파플랜 P15A 포터블</t>
+          <t>삼성전자 스마트모니터 LS32BM801UKXKR</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>179,000원</t>
+          <t>548,990원</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1,282개</t>
+          <t>399개</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>https://cr.shopping.naver.com/adcr.nhn?x=WK%2F2EedJLzH5WnX97nHKNf%2F%2F%2Fw%3D%3Ds40SCG98nN7bdmq4lUIyzcNy4K1pNtS0Don73smnYv6P6D9Doef8fQXU6eDjUh3hFKDYfPvQTIRxjKRPkqTYwXY4WQBe%2FZFkvs1gZ836hbpCe2umHfF2aLgG%2F437Vl%2B2i%2Br%2FdgAtqVYj6DoA7Mm4WZMv%2BjB2erv%2BZ%2Brrs5VHOiTQgGE7%2BZatKjf5hEf1XctkKe98HYwHRohe%2BaZU4HHRF1ZnNrwRClxwG6KI6Xy%2BWtBSkj8Xd80xPWZvn6URexO9BvdrxPgprIfciPgkJT4vsx0Pg%2F6PYJW9LpCSumzPJoigK7CtQzZWLlur1%2FFge4%2BEpl7NMO5kb9qju5W1nChDiiF9YBnCgL9Blqo%2BU00aSWNakudW4LAgR4Xxl%2FdcF1QLKSz17DC0z8j15Nwxy%2FSN4aT6FURihOvVNK6%2BarovFEXZwoG%2BQ0x2bZ6nINFkvNJO6TFPtDewCXlQKpMr%2Be9cSobuyhUYb3VXENZjLt59b%2BWA3THpYa%2BgjQe1jwgPp6enXPNRouOLVBR9bkVCm5wEj0Hs3T4qzSBIVN2HAysFdoOTkx%2Fj3RBe3arV4wSkm4%2FnrhqXa5jOS8gZiCn0A0UB7Jw4SwcLvxUEucVmH%2BcOht40%3D&amp;nvMid=20651265453&amp;catId=50000153</t>
+          <t>https://cr.shopping.naver.com/adcr.nhn?x=%2Ft%2BWtOYDzmzlHkpElUT03%2F%2F%2F%2Fw%3D%3DsQXGmADXHdKMrYIk71LPZ8Ul0DPGldu4dRCaCLbT4fHlQ3qrx3p0MRIb3ekawSdvJZwaTXBSSMgH10Q4fP807YHfbiCgZda7QnETYwxJl1gGJJ%2Fc0J%2BnoHzQ97jNNHE%2FTaQaOQnHcjvvda2yBa%2BUJJd9%2BKy%2Fm0d%2BgYWHtEf61Jo5CNclKwvLyA%2Fys%2F%2FHPPajLph32Ku4C8WdFP0IDZI%2FGziKH4uGhdMZI%2BTAm7Oh3XZYWq6062OEPPa9WB%2BtWbtCGjgKe6djeuWuGZllC7f3Jz6sJF1TG8DXvuOXRWh2aiSE1QmeK3ZPITzKHcbEnR%2BI87b%2B5QWa2rqHG3KeTA4jap%2BLeQ6PxCXBM%2BK%2BSNPfmpbRXfqiCwBtPYYwEdSt6i2JAYMKIjKYePmwuWsaOUHOf%2Fw680anrzfzPbA%2FhSANHim0mBDonngitmc0jKl7CBWyu1kANx%2BCBziiow5%2FppcqS%2BVxnymBMau7huBRiFGHDzbE5K3vijH5wpE2U7NlKb5LGe%2BT6TT5Bsxcst6fViWwYQo6%2F74bs%2FzNmznhIO5N5zjUkqRWr%2BdA5itkX2Tq2NXXdeaK8Ljlt0Axb7DbuUT%2FK72hopkeKUdu5q4dSKA0zkoA%3D&amp;nvMid=31160861618&amp;catId=50000153</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>삼성전자 스마트모니터 LS32BM801UKXKR</t>
+          <t>제우스랩 알파플랜 P15A 포터블</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>548,990원</t>
+          <t>179,000원</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>399개</t>
+          <t>1,282개</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>https://cr.shopping.naver.com/adcr.nhn?x=IxOUo%2BZCipen0hXKPlv9z%2F%2F%2F%2Fw%3D%3DsQRYD1GhHKYzcJBuDEQVXuMrLOtVEqDw1ZhAmkgyCuAn6D9Doef8fQXU6eDjUh3hFS663piFm753Ay%2B108YlUTI4WQBe%2FZFkvs1gZ836hbpCe2umHfF2aLgG%2F437Vl%2B2i%2Br%2FdgAtqVYj6DoA7Mm4WZMv%2BjB2erv%2BZ%2Brrs5VHOiTQgGE7%2BZatKjf5hEf1XctkKe8ppXZHxmCxty6d249mTKJnNrwRClxwG6KI6Xy%2BWtBSkj8Xd80xPWZvn6URexO9BvdrxPgprIfciPgkJT4vsx0Pg%2F6PYJW9LpCSumzPJoigK7CtQzZWLlur1%2FFge4%2BEp6%2BiBgH9abZzKnk3OPDqRWrXYOjtn2xi6MzYEOhwHwUGkudW4LAgR4Xxl%2FdcF1QLKbbAWHDnVl94XpFW9tJ94Yt1woZLwre%2F0c6LfC8XQvOYzOshqLKJjeTGrYo5ReDfbsI5P%2FndL7Fk2zkYLWAMRXbuyhUYb3VXENZjLt59b%2BWCbL%2F15f%2FdVKXhm1xsU9UOUdRM2ejeXMHLKUhaOgGkIEo%2F2jOZ1X9azl5NH1VOMKFuDJB3Kc9QHlBEzTDa81EKDGfsQNiPhdh19R%2BWbND42xw4SwcLvxUEucVmH%2BcOht40%3D&amp;nvMid=31160861618&amp;catId=50000153</t>
+          <t>https://cr.shopping.naver.com/adcr.nhn?x=1C1LH8hlRHiDhDJyUMBaCP%2F%2F%2Fw%3D%3DsIH%2BzQyHVHoT8fnBQbGCdsR8Wjank9VdcwJnjKGrOvfNQ3qrx3p0MRIb3ekawSdvJflnFpAEnTycFrY3YyTMrKnfbiCgZda7QnETYwxJl1gGJJ%2Fc0J%2BnoHzQ97jNNHE%2FTaQaOQnHcjvvda2yBa%2BUJJd9%2BKy%2Fm0d%2BgYWHtEf61Jo5CNclKwvLyA%2Fys%2F%2FHPPajLQahfztBy%2FxYsI%2BwV0HuB3iKH4uGhdMZI%2BTAm7Oh3XZYWq6062OEPPa9WB%2BtWbtCGjgKe6djeuWuGZllC7f3Jz6sJF1TG8DXvuOXRWh2aiSE1QmeK3ZPITzKHcbEnR%2BI8UKV3ZzeG7JzEkP9GbJCBseSv%2BU6FXGPNGPgp4dTHtQdXfqiCwBtPYYwEdSt6i2JAzcOFBHPtzvb5Oyfxxc%2FgAzECHSOrHCGaqKmefk7cLnvInLOBdmwThx8QczlsqpkY2%2BPFdbKtLo%2FXpqGntaFLF1xnymBMau7huBRiFGHDzbEGZA4k8IHYppYoYfXJIfgYSa9PrgMXmjA5cn%2BtnfHJjI6%2F74bs%2FzNmznhIO5N5zjVQRCoZndbVQk3qHp%2BKZUwh3iBEcMN1BXDxy7w%2Bc21QZWhopkeKUdu5q4dSKA0zkoA%3D&amp;nvMid=20651265453&amp;catId=50000153</t>
         </is>
       </c>
     </row>
@@ -907,7 +907,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>https://cr.shopping.naver.com/adcr.nhn?x=YCVydqhWhRNGYwodLwRuX%2F%2F%2F%2Fw%3D%3DsKZUce07giSFmRwsqSZwnwm%2BY7vrCxIZCEFGbmrZH0FLkEFD9EqEzeuo8lvy6ZeyvJxQKllR7W0BesfOYDSYyKlUDpZsgzFAFORfT0UtaVWZ7h4YxfqVFkPRVarjF1EJTLI7AZ9LZDmHnAQwsi59Cc1Vd6Z%2BmZ5fvTALbBBPmfKJ6LYABWm6lRkxVNeHofoG1OFjM5yt680g30OYA7rP3zCkbYBqhSVo%2BVMrTfeSHmNZ0UYwtLvFUZlvWLdyGP2oVcBtQ3uJLcsd%2BBJyrtZXBtcOmY27ZGze0Q%2BtXRlM4OxtarJoVrbEtunAYIkKGowOqJuS%2BtOK4tptCZ68hRVZ%2FaCEhb%2B5%2BbgCLWD5ufmjwVaBxgrKyGzgTjgvZMIoXgNJhsCPTKAShkHrDCK20b55m5qAhfbmRc6T9Q91MqoVII6qwx8fmV2SoX8VoStIDaYcCdLM%2FEvjrD3XSrLys71wSXnjXlqeOuEAxULqnTRomXy6co%2BEgeOt%2FGgTaW1PsDX8qAYTYOqTv%2FsOm0kcFv3bjpC6zeBVuJ%2F1kiunwa7a4AQLftrNaoHZF3j6ZGLWRnluyb1NmOoRBMBsXNQGXzjfbC%2BFUQB%2FrDAzm2q1KHRsHkfE%3D&amp;nvMid=31605356618&amp;catId=50000153</t>
+          <t>https://cr.shopping.naver.com/adcr.nhn?x=aMEXE5mEiK0o4mZGXZnu2f%2F%2F%2Fw%3D%3DsHIi2rhGFHxvzgRRoBG75LZhWm7cVcpW9N3h7PXBuGrVQ3qrx3p0MRIb3ekawSdvJOBcbj1ZI7kjQLrbWQUnDO3fbiCgZda7QnETYwxJl1gGJJ%2Fc0J%2BnoHzQ97jNNHE%2FTaQaOQnHcjvvda2yBa%2BUJJd9%2BKy%2Fm0d%2BgYWHtEf61Jo5CNclKwvLyA%2Fys%2F%2FHPPajL80wuX%2BWwruX9jqelNfBuuiKH4uGhdMZI%2BTAm7Oh3XZYWq6062OEPPa9WB%2BtWbtCGjgKe6djeuWuGZllC7f3Jz6sJF1TG8DXvuOXRWh2aiSE1QmeK3ZPITzKHcbEnR%2BI8KS0%2Ft0tLRxBXYfIQlwOwFH%2BOjRn6NEcyO9tdH4U1v%2BlXfqiCwBtPYYwEdSt6i2JAYyECQ14BLlqI0u8jnppJ0wjz9k9vTGDZJcRCmwirAOgYtq2ME1Xm1HVm1yx1p5EzGMNmFgB8Ru97e8xqUMKQAbuyhUYb3VXENZjLt59b%2BWCdnmiyA6MTzRDL5MVyWm%2FcPNRouOLVBR9bkVCm5wEj0I%2F2jOZ1X9azl5NH1VOMKFv3iiogFOk0pwCmCWpDflJlJ5afp0An30RQ1Hl0SAib4Q4SwcLvxUEucVmH%2BcOht40%3D&amp;nvMid=31605356618&amp;catId=50000153</t>
         </is>
       </c>
     </row>
@@ -929,7 +929,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>https://cr.shopping.naver.com/adcr.nhn?x=9GyI76hceCMEXeC4Sc4Juv%2F%2F%2Fw%3D%3DsclB16uwxHc3%2B5LQxFQ77emijdBf20qgvrBhkHLon06b6D9Doef8fQXU6eDjUh3hFc2qDG32OvJrOPZrbaOzylY4WQBe%2FZFkvs1gZ836hbpCe2umHfF2aLgG%2F437Vl%2B2i%2F5EF1HLjMga4CxGmmb%2B6L8VIhUTYq2J1wF4XcKD2AOWkOA3ZateG%2FY8eKxwX1E0NnLvwmv6hWhMH5BqHNDglFHAbUN7iS3LHfgScq7WVwbXDpmNu2Rs3tEPrV0ZTODsbWqyaFa2xLbpwGCJChqMDqpjVoW2AknYreBXSAebSaNqSS%2Ff2riZoUlTfhdh5lbGc6qZE9VDyiNqUU0Ox5CBvZER3QaSOv88j%2Fcuimj1AovTN81WjUpxJVJrN5mDsz4BpFoHVr0oyndyMMRpXo4lVD7Kfm5oam2WJXcpaxc1jwE6tPbqZ1%2Fyra9AKyn8MsBMma8jdKDgmGaMnuKqZNdPrso%2Bbl8ZyzU49%2BSpAijorRdICIu%2B0VjoXZPNoiNaFTjewlbneYUIh4AeIj88oRCJD3gFAtjRv%2FqLUyuG2DIqEBXWSkaO7edYhsb7H23VMSQM0WFCYHlb7IWxdvry9Xf7Bx33x1kV%2Fgds54fkDY4hiMQpvU2Y6hEEwGxc1AZfON9sL4VRAH%2BsMDObarUodGweR8Q%3D%3D&amp;nvMid=82278580434&amp;catId=50000153</t>
+          <t>https://cr.shopping.naver.com/adcr.nhn?x=89JttNBkOdRlswgA0b6eKv%2F%2F%2Fw%3D%3DsRahN6x3OBAqGtejbPLtrPGijdBf20qgvrBhkHLon06b6D9Doef8fQXU6eDjUh3hFwcCplbR91EgkSvUfMC5VG990lYqjsgb%2Flwx642gSpssQKb3gny%2BhmcHehTHkI9Y9lXiENlhoM2unyEV278%2BIVcVIhUTYq2J1wF4XcKD2AOWkOA3ZateG%2FY8eKxwX1E0NnLvwmv6hWhMH5BqHNDglFHAbUN7iS3LHfgScq7WVwbXDpmNu2Rs3tEPrV0ZTODsbWqyaFa2xLbpwGCJChqMDqpRBPzLxAXYvZHQW%2FtOLIQCSS%2Ff2riZoUlTfhdh5lbGc6qZE9VDyiNqUU0Ox5CBvZER3QaSOv88j%2Fcuimj1AovTN81WjUpxJVJrN5mDsz4BpFoHVr0oyndyMMRpXo4lVD7Kfm5oam2WJXcpaxc1jwE6tPbqZ1%2Fyra9AKyn8MsBMma8jdKDgmGaMnuKqZNdPrso%2Bbl8ZyzU49%2BSpAijorRdICIu%2B0VjoXZPNoiNaFTjewlbneYUIh4AeIj88oRCJD3gFAtjRv%2FqLUyuG2DIqEBXWSkaO7edYhsb7H23VMSQM0WFCYHlb7IWxdvry9Xf7Bx33x1kV%2Fgds54fkDY4hiMQpvU2Y6hEEwGxc1AZfON9sL4VRAH%2BsMDObarUodGweR8Q%3D%3D&amp;nvMid=82278580434&amp;catId=50000153</t>
         </is>
       </c>
     </row>
@@ -951,7 +951,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>https://cr.shopping.naver.com/adcr.nhn?x=hKHU3i67EBfBDKA6EIsXd%2F%2F%2F%2Fw%3D%3DshC68CryW0%2FrjCEWClwzce09ANXq0z5KbndR6W1zoJXX6D9Doef8fQXU6eDjUh3hF0vdTJJwZTu0fvpEns5k%2BYI4WQBe%2FZFkvs1gZ836hbpCe2umHfF2aLgG%2F437Vl%2B2i%2Br%2FdgAtqVYj6DoA7Mm4WZMv%2BjB2erv%2BZ%2Brrs5VHOiTQgGE7%2BZatKjf5hEf1XctkK7UgVakcvYnJL8a%2B%2FTtLoWZnNrwRClxwG6KI6Xy%2BWtBSkj8Xd80xPWZvn6URexO9BvdrxPgprIfciPgkJT4vsx0Pg%2F6PYJW9LpCSumzPJoigK7CtQzZWLlur1%2FFge4%2BEprkfC1B39rsHol743tV4Xhv0PqpzS9bsPbua3QvdT2KOkudW4LAgR4Xxl%2FdcF1QLKBOJIWjfBKb72VxkRy6VvUd1woZLwre%2F0c6LfC8XQvOYGsxBcpcj%2Bn0m4NCRLi2SBwoHcdukJ3JwXOF8ho9HQSAqrRpvIAQZSvQnJJtRel5rkCAnqiOYciFHVNJdQGNFhwtIYh35n85gCNF9XAudNirBvjyDto1XW7ogw3FQazkz%2Fhb06lCNf9EHWalJY3vi5owGYMReyNF5wktXeJqGcjUHQIiXcF4qwUXZ2sX76wW8%3D&amp;nvMid=31889649618&amp;catId=50000153</t>
+          <t>https://cr.shopping.naver.com/adcr.nhn?x=%2F6SCZd82HYh8ooFYv5vpKv%2F%2F%2Fw%3D%3DsQqBpamsWUifadKnDqIgIcNuZ04OF9q4g7I5yXmci%2F%2BdQ3qrx3p0MRIb3ekawSdvJBwOshA%2BpuqzSOeF8kLQhjXfbiCgZda7QnETYwxJl1gGJJ%2Fc0J%2BnoHzQ97jNNHE%2FTaQaOQnHcjvvda2yBa%2BUJJd9%2BKy%2Fm0d%2BgYWHtEf61Jo5CNclKwvLyA%2Fys%2F%2FHPPajL5Dcpssy6IQFj1%2FMzORAPUCKH4uGhdMZI%2BTAm7Oh3XZYWq6062OEPPa9WB%2BtWbtCGjgKe6djeuWuGZllC7f3Jz6sJF1TG8DXvuOXRWh2aiSE1QmeK3ZPITzKHcbEnR%2BI8Aw4h8wxINR%2Fqmz2nzH58JDkLfbebuqnhLJojB8Bvjs1XfqiCwBtPYYwEdSt6i2JAZYHoE14ForuTOpcXp6PZRx2pl2tyBzXWWRZDIoC4zPwYtq2ME1Xm1HVm1yx1p5EzV%2BFiF9tPEaACBzpIQFCWPruyhUYb3VXENZjLt59b%2BWB%2BpFio96f4scWlNfoMTdhZccZSz1EueDaSgf%2BZjnoS0Y%2F2jOZ1X9azl5NH1VOMKFuL3O44sixaZjczulVcWX6eotPPrEbwnciWXOgQKHvYqQ4SwcLvxUEucVmH%2BcOht40%3D&amp;nvMid=31889649618&amp;catId=50000153</t>
         </is>
       </c>
     </row>
@@ -973,7 +973,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>https://cr.shopping.naver.com/adcr.nhn?x=Eif3C5nIPxuDRCrb0w9tJ%2F%2F%2F%2Fw%3D%3Ds%2F0%2BcGZcsgP%2FX8Wnzwuq2pBU6sUw%2FwVc3JSNmwlByCGzkEFD9EqEzeuo8lvy6ZeyvnFRYxQ7p%2FmPPgMqqp5GM0lUDpZsgzFAFORfT0UtaVWZ7h4YxfqVFkPRVarjF1EJTLI7AZ9LZDmHnAQwsi59Cc1Vd6Z%2BmZ5fvTALbBBPmfKLSnb5TTG5Ask4ivDxm9zzm%2FHJNUk%2Bhb5ztlxDJofRv0CkbYBqhSVo%2BVMrTfeSHmNZ0UYwtLvFUZlvWLdyGP2oVcBtQ3uJLcsd%2BBJyrtZXBtcOmY27ZGze0Q%2BtXRlM4OxtarJoVrbEtunAYIkKGowOqU8%2FX0ycn378WgsyYFBL%2BhSEhb%2B5%2BbgCLWD5ufmjwVaBxgrKyGzgTjgvZMIoXgNJhRqEa%2BcKqb7DId6RNjIcPwKAhfbmRc6T9Q91MqoVII6qp4xP7VJZgsIUqlVe4M9Iqo64ifB9DVeZ8ffla9GlFdlQckdnw8roVuf0XlEJ03gK%2FRhRXFpTt2%2FCbOS1hQrG%2BYnHIcETcJifOE8sb44IMxQYqCEuqwpxe6i9jDxqeX2XbU66vqpH6bVcE2P6FhWpJ5Hv1T%2FoDPeAT2ZD%2BWCfnsQ%3D%3D&amp;nvMid=38608938618&amp;catId=50000153</t>
+          <t>https://cr.shopping.naver.com/adcr.nhn?x=DAiU3WJ93%2BzKGjckmctXg%2F%2F%2F%2Fw%3D%3Dsv6Orpkvl%2F3T1MzeCOLqm64Qm4NXP2zPYpvcVgmOWAhxQ3qrx3p0MRIb3ekawSdvJwV9kGMG1zV5G0wqLOCoaf3fbiCgZda7QnETYwxJl1gGJJ%2Fc0J%2BnoHzQ97jNNHE%2FTaQaOQnHcjvvda2yBa%2BUJJd9%2BKy%2Fm0d%2BgYWHtEf61Jo5CNclKwvLyA%2Fys%2F%2FHPPajLjlhaM75gEzFLkm67xy1IoCKH4uGhdMZI%2BTAm7Oh3XZYWq6062OEPPa9WB%2BtWbtCGjgKe6djeuWuGZllC7f3Jz6sJF1TG8DXvuOXRWh2aiSE1QmeK3ZPITzKHcbEnR%2BI8l0JesmmM9kmID5Lt%2FuuknONGnrc1PtYLOFEAmtmQ1PNXfqiCwBtPYYwEdSt6i2JAA4EfR23DeIWfI88UdYfKVRSGVW6ii5yAOLexHrDf362ITF%2Bn1aaTvXziEq%2F4Mxnv5UZ0TKYQZku7MFsX2G5Zs1BvIAaonlqWGjb4wlVZ4pThtkS8543gTpUucry%2F7%2B2nT%2BDzDxwp7nT02YxkVA94lKrgl5lz2ILpWJJ%2BdahOgOJbUMI%2FoZ0WDfSTZWSX2NmzX45HjZZF2gj6d4jFl3EbsQau4fTwOUqyF63FjwpQRls%3D&amp;nvMid=38608938618&amp;catId=50000153</t>
         </is>
       </c>
     </row>
@@ -995,7 +995,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>https://cr.shopping.naver.com/adcr.nhn?x=fkkI%2BlUNZk5REDsuX6Or5%2F%2F%2F%2Fw%3D%3DsbUW0gPXVRPcPlqgbYrealC0gt5KcCMVaEP2QBcBwbtj6D9Doef8fQXU6eDjUh3hFWEDHTF1QrrsE%2B%2BKiq0qAs44WQBe%2FZFkvs1gZ836hbpCe2umHfF2aLgG%2F437Vl%2B2i%2Br%2FdgAtqVYj6DoA7Mm4WZMv%2BjB2erv%2BZ%2Brrs5VHOiTQgGE7%2BZatKjf5hEf1XctkKnMzmrUq%2BW8NPpwtsruY%2BD5nNrwRClxwG6KI6Xy%2BWtBSkj8Xd80xPWZvn6URexO9BvdrxPgprIfciPgkJT4vsx0Pg%2F6PYJW9LpCSumzPJoigK7CtQzZWLlur1%2FFge4%2BEpHEysJOMLfL8%2FAW9E%2FYwEtIRQPUXhUiTNC9Gsou6VEWKkudW4LAgR4Xxl%2FdcF1QLKnMBa%2F6Cmr72C3k%2BgyyILbLL%2BD79JFqXUHChswIKAa5dG4QUnlcoUG02XUvJNW82Ax8%2F6BemueUyNMp501BFwUP4x4I6qIyxidauif88nFTFAhf0nKlpB%2FPRgYb5y4WJ%2FnUpTzmQTeleeE0y%2Brv8xbDVx%2F1SAN%2F82L3SBPp6Pki006DwlaXBS8wbvh7aeyxJgA35CyMrpXQUt3%2FJvHupy5s1ITc7NlRPvorKrNyQBKaY%3D&amp;nvMid=23849172522&amp;catId=50000153</t>
+          <t>https://cr.shopping.naver.com/adcr.nhn?x=Nmbv9QO3oz8IwJAOlw3gGf%2F%2F%2Fw%3D%3DsSZfKTbE6D7Cewgtxj5DFWC0gt5KcCMVaEP2QBcBwbtj6D9Doef8fQXU6eDjUh3hF7yP%2BScwPt05uy9fCvdHBNd90lYqjsgb%2Flwx642gSpssQKb3gny%2BhmcHehTHkI9Y9gm95oC2yEe6xrBnXD61GF8v%2BjB2erv%2BZ%2Brrs5VHOiTQgGE7%2BZatKjf5hEf1XctkKnMzmrUq%2BW8NPpwtsruY%2BD5nNrwRClxwG6KI6Xy%2BWtBSkj8Xd80xPWZvn6URexO9BvdrxPgprIfciPgkJT4vsx0Pg%2F6PYJW9LpCSumzPJoigK7CtQzZWLlur1%2FFge4%2BEpJB7WazZY%2Fl5q9WHbyJ%2FG4Zywmfj8NdAhanNCimhlftekudW4LAgR4Xxl%2FdcF1QLKnMBa%2F6Cmr72C3k%2BgyyILbLL%2BD79JFqXUHChswIKAa5dG4QUnlcoUG02XUvJNW82Ax8%2F6BemueUyNMp501BFwUP4x4I6qIyxidauif88nFTFAhf0nKlpB%2FPRgYb5y4WJ%2FnUpTzmQTeleeE0y%2Brv8xbDVx%2F1SAN%2F82L3SBPp6Pki1r3bhGCOUbIl%2BGpYdeCIqLA35CyMrpXQUt3%2FJvHupy5s1ITc7NlRPvorKrNyQBKaY%3D&amp;nvMid=23849172522&amp;catId=50000153</t>
         </is>
       </c>
     </row>
@@ -1017,7 +1017,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>https://cr.shopping.naver.com/adcr.nhn?x=NE597lko7CP2xLD%2BTZousP%2F%2F%2Fw%3D%3DsePLS4numGpLdbTbckRBNcimAZiC0XKTLrnhsYdz1LdpQ3qrx3p0MRIb3ekawSdvJTb%2BhEhutovTKTv8Qohic2jF58jfAIBSb%2BHVg6fYTWJTOBrkH5eL%2BGiYgkRcbqqAc3bHOcygeCu4ZWtd%2FrJCted9%2BKy%2Fm0d%2BgYWHtEf61Jo5CNclKwvLyA%2Fys%2F%2FHPPajLQrDsk0DFY%2FKP0N6xxzqd%2FSKH4uGhdMZI%2BTAm7Oh3XZYWq6062OEPPa9WB%2BtWbtCGjgKe6djeuWuGZllC7f3Jz6sJF1TG8DXvuOXRWh2aiSE1QmeK3ZPITzKHcbEnR%2BI87z74NtkDPVVoBquUVTc7eMaKhEGr%2BoXEnQhQk2C8o11XfqiCwBtPYYwEdSt6i2JAWCVDFxbY5SHUOYc%2Fa%2Fe3iJodd6dHeZDGvCrbcHhTGm17r%2FEca5hWftYoIO0zsH%2FmtlESLGBuREG1DpgWtFtEQrKHULBFwaApMjsVr%2BJOmv%2F2xXLMavbAM5rpgiaUg2%2BfwtIYh35n85gCNF9XAudNigvhUoceLrljqEXFuG61rqu9zSNGmYjO6hioKvVWCmnVPuzp1uzMcXa76Rrv4%2B0bMkHQIiXcF4qwUXZ2sX76wW8%3D&amp;nvMid=22483121542&amp;catId=50000153</t>
+          <t>https://cr.shopping.naver.com/adcr.nhn?x=25zO1wsiNb7jif%2FkATb06f%2F%2F%2Fw%3D%3Ds1AcREnNlTGvs5UP%2BIkfLjSI0OEbS%2FQrznpgIqouxf7T6D9Doef8fQXU6eDjUh3hFUqs6BFhLACQZKLHsmBOtid90lYqjsgb%2Flwx642gSpssQKb3gny%2BhmcHehTHkI9Y9gm95oC2yEe6xrBnXD61GF8v%2BjB2erv%2BZ%2Brrs5VHOiTQgGE7%2BZatKjf5hEf1XctkKkFJ709UOTEZ7t%2Bo%2FJTVy6JnNrwRClxwG6KI6Xy%2BWtBSkj8Xd80xPWZvn6URexO9BvdrxPgprIfciPgkJT4vsx0Pg%2F6PYJW9LpCSumzPJoigK7CtQzZWLlur1%2FFge4%2BEppu%2FJQwpN9ifcRb7IMxcDwrlJH1q0EGOKact1MGcMYxKkudW4LAgR4Xxl%2FdcF1QLKcOkdkdbNaRKpuVQl2fvr5rL%2BD79JFqXUHChswIKAa5cb74AQf40n6QSZcJbWQRA8UgDeNNUDg9e%2BWhGTM057mGwXJTrdVSZiRku5ZQPk%2F0fAkrCP%2BzeIIohumyxQWoCEAYTYOqTv%2FsOm0kcFv3bjpKDKKHRfeF42dMQ9RycXGAZzguJfe3UUmXjaN8KtUKwdb1NmOoRBMBsXNQGXzjfbC%2BFUQB%2FrDAzm2q1KHRsHkfE%3D&amp;nvMid=22483121542&amp;catId=50000153</t>
         </is>
       </c>
     </row>
@@ -1029,7 +1029,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>186,510원</t>
+          <t>186,300원</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1039,7 +1039,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>https://cr.shopping.naver.com/adcr.nhn?x=994IgOVVlb%2BzgXUjDkC7XP%2F%2F%2Fw%3D%3DsIki7NxfBVlmTL4fFbZRJjMT6F7c6UaFD%2FNkyk4c4JXD6D9Doef8fQXU6eDjUh3hF3UfvriNtlSxI5WcqH40%2BRI4WQBe%2FZFkvs1gZ836hbpCe2umHfF2aLgG%2F437Vl%2B2i%2Br%2FdgAtqVYj6DoA7Mm4WZMv%2BjB2erv%2BZ%2Brrs5VHOiTQgGE7%2BZatKjf5hEf1XctkK9H2Ry0j4gqCp%2FslqlW6BdJnNrwRClxwG6KI6Xy%2BWtBSkj8Xd80xPWZvn6URexO9BvdrxPgprIfciPgkJT4vsx0Pg%2F6PYJW9LpCSumzPJoigK7CtQzZWLlur1%2FFge4%2BEpHbKIHqPGuuJgLDfc7PHT8jyxWhQRjlqjDrwCeNeTiaOkudW4LAgR4Xxl%2FdcF1QLK0gQSX9HERKpAs5r6tMgfmd1woZLwre%2F0c6LfC8XQvOYAvSZCVxfLmJeWFo%2B3ljwuZrzhsr6pANGTPCAkiEySKJoCT2VnN3qw2jqjy5A%2BjrGFMQasWwRYVRBFQScxhWrcnUpTzmQTeleeE0y%2Brv8xbFBLcHc2bKrqxy3gUczGDtKLYgK4qPfAXmKYiSLRxiIgA35CyMrpXQUt3%2FJvHupy5s1ITc7NlRPvorKrNyQBKaY%3D&amp;nvMid=36645769618&amp;catId=50000153</t>
+          <t>https://cr.shopping.naver.com/adcr.nhn?x=GCHeWEArbLDJHDE28VSaQf%2F%2F%2Fw%3D%3Ds0goS%2BaXwpiVFxadxcOLcI5rPlBtbh13LxxFZ1%2FbTnXVQ3qrx3p0MRIb3ekawSdvJ3OiD9ck5Yq10jfWtsH6r03fbiCgZda7QnETYwxJl1gGJJ%2Fc0J%2BnoHzQ97jNNHE%2FTaQaOQnHcjvvda2yBa%2BUJJd9%2BKy%2Fm0d%2BgYWHtEf61Jo5CNclKwvLyA%2Fys%2F%2FHPPajLlIuyWsBMEk%2BMjpqdwEGjkSKH4uGhdMZI%2BTAm7Oh3XZYWq6062OEPPa9WB%2BtWbtCGjgKe6djeuWuGZllC7f3Jz6sJF1TG8DXvuOXRWh2aiSE1QmeK3ZPITzKHcbEnR%2BI8NYTKSYvvtXTM6Ns2CYM2QB4s7S126sG7CBnlbFhiX2NXfqiCwBtPYYwEdSt6i2JAzUiAS1WE3SdEJRglravs1B2pl2tyBzXWWRZDIoC4zPw2J9uOr2XC1EimviKxbk1XSZU5J7o15pK1Wb0cuM%2Bc0sHZEvwaUbBiDy0QqT%2Bd0Cy8EHfc6fQwSmmWkU4ofUI2T%2BDzDxwp7nT02YxkVA94lCqAQZy8wU1H8Lc%2FRXdx9IzM9hPIIhaZB9mlrcsLdEgftPzsxdK21zCUMX7TCc3PLgau4fTwOUqyF63FjwpQRls%3D&amp;nvMid=36645769618&amp;catId=50000153</t>
         </is>
       </c>
     </row>
@@ -1061,7 +1061,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>https://cr.shopping.naver.com/adcr.nhn?x=CQ6Q2NqG7eRoM%2Bg%2B3w8Nbf%2F%2F%2Fw%3D%3DsMnSxyXgbA5dKZtigYldGweO4cy0JufM3I9qZd%2BMpo6v6D9Doef8fQXU6eDjUh3hFMH5T5A28awd9tL1zoAQGEo4WQBe%2FZFkvs1gZ836hbpCe2umHfF2aLgG%2F437Vl%2B2i%2Br%2FdgAtqVYj6DoA7Mm4WZMv%2BjB2erv%2BZ%2Brrs5VHOiTQgGE7%2BZatKjf5hEf1XctkKeuRhUvw6XywB6YV5N8362pnNrwRClxwG6KI6Xy%2BWtBSkj8Xd80xPWZvn6URexO9BvdrxPgprIfciPgkJT4vsx0Pg%2F6PYJW9LpCSumzPJoigK7CtQzZWLlur1%2FFge4%2BEpj0XdymX4vS810zEsRvPvL76tiOPWuWMQDG9OLlu9axukudW4LAgR4Xxl%2FdcF1QLKsODix3xe7w%2Bfc3QNpjKYvdwRQyT5iDRlXdtlKXilPLJmGZQoVV7tYtN3LGMG2W2KoLEA4enSeMpYZPphZ8YeEon8Hd7Ei%2BzPNsLiDE9G1JdfPiIoEK%2FIqU85bpPstA04UTeuJgZvRvEK7gZCw3B0%2BinOk7Kb%2BlQZIR3dDuO0sISNCPgQ02Sxvd4iOKclrKlaY7RBJx2aPv1bgiR77Jh46w1QmAmnoJRdq4K9btjkCM0%3D&amp;nvMid=23244797490&amp;catId=50000153</t>
+          <t>https://cr.shopping.naver.com/adcr.nhn?x=5Gi0u10P8cOMqm7KxVv9kP%2F%2F%2Fw%3D%3Ds3JW6PKeyIaJrUAhEtZ%2B050Et76LNKLZg58oQROKVLNLkEFD9EqEzeuo8lvy6Zeyv4TgJWrCazpKOfit080d0jw2CWj34psFuHU6FoG79mLHoxqQvhEGfzIuiGTUnSeUQIxXmfNKpE7CUL7F3u6%2B2DlVd6Z%2BmZ5fvTALbBBPmfKL%2BHMhXfuiFC4uELuwCB7Zjn0PJUDtK%2FaNCzmEqks6RFSkbYBqhSVo%2BVMrTfeSHmNZ0UYwtLvFUZlvWLdyGP2oVcBtQ3uJLcsd%2BBJyrtZXBtcOmY27ZGze0Q%2BtXRlM4OxtarJoVrbEtunAYIkKGowOqE8jGR%2Fifg2aICklLHNzAXCEhb%2B5%2BbgCLWD5ufmjwVaBxgrKyGzgTjgvZMIoXgNJh%2BAIDPyQbRo%2F2m49LAFa4LaAhfbmRc6T9Q91MqoVII6oL1yJcw7BIb5wEpmsCyUJV9r2S1a7atr4GEfeU1LoItYAX23i%2FdrO0Ua0ezc8yIJpVHkSPxKP9dgMmoZ%2FKUx02DWrhHEcp0p%2F%2FKKziu53PdOvHmBY4LHQOQCLp1XD7evA%2FQR0oQ2IQYxEcIqISxWQ5VoWd0jB03C5aYq3HUc1IKtSSLJQZncWk8e8Ttfjz6Fs%3D&amp;nvMid=23244797490&amp;catId=50000153</t>
         </is>
       </c>
     </row>
@@ -1083,249 +1083,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>https://cr.shopping.naver.com/adcr.nhn?x=06rrTReoa%2B2PpLsZhxcT8P%2F%2F%2Fw%3D%3DsPJengRrT%2FR1gcMZ6b7wn%2FCQfgZwCAWeojltcUZSyPV76D9Doef8fQXU6eDjUh3hFfY3XjzAbsHuGBVy8GwfQQI4WQBe%2FZFkvs1gZ836hbpCe2umHfF2aLgG%2F437Vl%2B2i%2Br%2FdgAtqVYj6DoA7Mm4WZMv%2BjB2erv%2BZ%2Brrs5VHOiTQgGE7%2BZatKjf5hEf1XctkK9qSKXgoi8oGbG2WVp3jxEpnNrwRClxwG6KI6Xy%2BWtBSkj8Xd80xPWZvn6URexO9BvdrxPgprIfciPgkJT4vsx0Pg%2F6PYJW9LpCSumzPJoigK7CtQzZWLlur1%2FFge4%2BEppvA3ygU1LM92LOiOAZC%2BmLXYOjtn2xi6MzYEOhwHwUGkudW4LAgR4Xxl%2FdcF1QLKWVzqUgdvCXmKg0W8CnHjKXzEWKIeSL8gCGko0muIXASpsBVMxBwX6oIWWdxUIiiXpqJykqIyDolEoVJ%2FMTE6pHIEOMyyDocZ9XLqN14mUSyjriJ8H0NV5nx9%2BVr0aUV2TsG9V1%2FA7%2FvBFoby9LtaxAd5tuM5ZrevXvYAbtXnelFicchwRNwmJ84TyxvjggzF%2Bs8iZixIWRLFY%2FAfUHJJEbvytzE0oBXC8c%2BwMwTZD%2F%2Fke%2FVP%2BgM94BPZkP5YJ%2Bex&amp;nvMid=18778755031&amp;catId=50000153</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>한성컴퓨터 TFG34Q10W 1500R 커브드 게이밍 리얼100 울트라와이드</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>299,000원</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>2,280개</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>https://cr.shopping.naver.com/adcr.nhn?x=doAjXKSAOPha2niD%2FpmcjP%2F%2F%2Fw%3D%3Dsdlf6dEuNZDi42MfImzd0qbHcAyJB3PzAvdbQgAbEuAz6D9Doef8fQXU6eDjUh3hFiWjwNuqDL9QJVrPiJJoGXo4WQBe%2FZFkvs1gZ836hbpCe2umHfF2aLgG%2F437Vl%2B2i%2Br%2FdgAtqVYj6DoA7Mm4WZMv%2BjB2erv%2BZ%2Brrs5VHOiTQgGE7%2BZatKjf5hEf1XctkKWR0ao9mrY56oOpR0CYbUbZnNrwRClxwG6KI6Xy%2BWtBSkj8Xd80xPWZvn6URexO9BvdrxPgprIfciPgkJT4vsx0Pg%2F6PYJW9LpCSumzPJoigK7CtQzZWLlur1%2FFge4%2BEpbDiGGYRWWYBf8QwqUzTE7az4Lv3Fd148nhhi5p8xnW%2BkudW4LAgR4Xxl%2FdcF1QLK0az9AnXgPICDoivIYW4q4nornTeMFMWI76yU7BvGjg6psBVMxBwX6oIWWdxUIiiXMSZ4UZzIuoqhNd5WVL9FoTDr9LVEx1KN1MbN0AIMMyndpyt33C4MUkvcTtGUs2M4Z28ZGSR7clSgBeyU1V7tZ10e0%2F7oUtw182DVYHDHcyWswP7hDcN4IRr%2BqZnzyTMlmebZ7ZSzdkaAGB0p%2BJqIW%2FoLRdeTzJJo5DQ5ovPMjEUcoU2RVzRFdum5hBbVcPmKbPkUFdM583YHEJuCzCpGcctVYavx%2B%2B8fWZa9SBc8rqM%3D&amp;nvMid=20889802847&amp;catId=50000153</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>한성컴퓨터 ULTRON 2460G PLUS 리얼 144 게이밍</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>139,000원</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>3,344개</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>https://cr.shopping.naver.com/adcr.nhn?x=ooRUpW%2Byf4dx5E0Qftygev%2F%2F%2Fw%3D%3DsmBP2%2FRWvLZaZouFD%2F42FkioC3ooIrnrCQEFw6%2BqdJE36D9Doef8fQXU6eDjUh3hF8CQFv9bA7x09fjybccfebI4WQBe%2FZFkvs1gZ836hbpCe2umHfF2aLgG%2F437Vl%2B2i%2Br%2FdgAtqVYj6DoA7Mm4WZMv%2BjB2erv%2BZ%2Brrs5VHOiTQgGE7%2BZatKjf5hEf1XctkKzg35FY8GnLaRmQtn47vIZpnNrwRClxwG6KI6Xy%2BWtBSkj8Xd80xPWZvn6URexO9BvdrxPgprIfciPgkJT4vsx0Pg%2F6PYJW9LpCSumzPJoigK7CtQzZWLlur1%2FFge4%2BEpoyDUYUEybr%2FQnmGS%2Fz3%2B6Wuze7Xynw1HKTiTwqLW8n2kudW4LAgR4Xxl%2FdcF1QLK5DGYyxhs19iyt0qj0pvn1twRQyT5iDRlXdtlKXilPLKPnD7hJV2J05mLBD5naU%2BlzbP6cEWicAVR%2FRpNX8bn3VVjo2ktg0sDCWAevGKHtFIfKkIqrJpQ0eF8eozNLpwGXx6siot2CfMCibd1aGet7R24FtHg8Zv3vc3gCQaKAGoNauEcRynSn%2F8orOK7nc90XKAZcFrHI1tjZuUkdmjy%2BOF3YN9EIwKElV%2FPKUIOBYRWhZ3SMHTcLlpircdRzUgq1JIslBmdxaTx7xO1%2BPPoWw%3D%3D&amp;nvMid=32237923620&amp;catId=50000153</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>벤큐 GW2780 아이케어</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>189,000원</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>5,453개</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>https://cr.shopping.naver.com/adcr.nhn?x=cU%2BfXpo4ibg8374y2voPp%2F%2F%2F%2Fw%3D%3DsTqKDKwVn1QopF2e%2Bcp%2BDJxLx%2BHnd6F5rC6QzuFW98aHkEFD9EqEzeuo8lvy6ZeyvdqvBgj5e8Pt%2FfpQnnCj7FFUDpZsgzFAFORfT0UtaVWZ7h4YxfqVFkPRVarjF1EJTLI7AZ9LZDmHnAQwsi59Cc1Vd6Z%2BmZ5fvTALbBBPmfKIp9xwiV%2FBhjEl1I0IRvcB6rwQxQefaWcwERchpjqmAvSkbYBqhSVo%2BVMrTfeSHmNZ0UYwtLvFUZlvWLdyGP2oVcBtQ3uJLcsd%2BBJyrtZXBtcOmY27ZGze0Q%2BtXRlM4OxtarJoVrbEtunAYIkKGowOq7Dpnn5tH1s3TQGOXxpdPqSEhb%2B5%2BbgCLWD5ufmjwVaBxgrKyGzgTjgvZMIoXgNJhECt1KiroNy1KFZkcKXNLEKAhfbmRc6T9Q91MqoVII6qjoQoSsEqSQ1AMwfWyh%2BymabX6FJTXpCjwPDvRbHbCyV0e0%2F7oUtw182DVYHDHcyXUKpDn5geTrrMDnuLePm7s3uPQNTCZ9wr%2FrixWl3LsXPoLRdeTzJJo5DQ5ovPMjEVfG2UkzKHzTr%2Fu8dQpSadTPDC67Xv30%2B7Md%2F3E43KJuMtVYavx%2B%2B8fWZa9SBc8rqM%3D&amp;nvMid=11846746201&amp;catId=50000153</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>삼성전자 오디세이 G3 S27AG300</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>267,990원</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>2,763개</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>https://cr.shopping.naver.com/adcr.nhn?x=V6Ees%2BlGmfgQb5EH8pT22%2F%2F%2F%2Fw%3D%3DsqFz%2FFzngNtOLhw0xLMwE4myAhUoNhaGJr%2BsUZ3ztBuL6D9Doef8fQXU6eDjUh3hFpDZPrx9gC3n2OqPnGAt6JY4WQBe%2FZFkvs1gZ836hbpCe2umHfF2aLgG%2F437Vl%2B2i%2Br%2FdgAtqVYj6DoA7Mm4WZMv%2BjB2erv%2BZ%2Brrs5VHOiTQgGE7%2BZatKjf5hEf1XctkKsfbl3KGs4%2BDFeAFl5q6KU5nNrwRClxwG6KI6Xy%2BWtBSkj8Xd80xPWZvn6URexO9BvdrxPgprIfciPgkJT4vsx0Pg%2F6PYJW9LpCSumzPJoigK7CtQzZWLlur1%2FFge4%2BEpUg7wM0jOOLtFesDogOH3yNI4ZgIWDIv50yvmBg%2FSOQOkudW4LAgR4Xxl%2FdcF1QLKd5uBS5N1d%2FL%2BdEvkr0hQobL%2BD79JFqXUHChswIKAa5fiatdtFnUSuHLhDUzB5UCEQEw6oyMRufRNxJLkl8x3OM%2F5hcznkGNop8Iw2jp0ykB3sK%2FDL95CrVUrbZEEaA89wtIYh35n85gCNF9XAudNiqpNffAH9QGJLz8lJt1xkPho%2Fldu9G3djcnA0N1CMQ51eyeOTkmw%2BlVMpsrSumNrFUHQIiXcF4qwUXZ2sX76wW8%3D&amp;nvMid=27535066522&amp;catId=50000153</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>LG전자 울트라HD 27UL550</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>398,790원</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>4,573개</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>https://cr.shopping.naver.com/adcr.nhn?x=ngljpudsr2G4gfwkziPDe%2F%2F%2F%2Fw%3D%3DsRZhUexsHsajx3QLA%2BNBwwo1Vxo3ixKdg6ab9J%2FQESwDkEFD9EqEzeuo8lvy6ZeyvRkDAnhiq0Dd6T1DNJxybjlUDpZsgzFAFORfT0UtaVWZ7h4YxfqVFkPRVarjF1EJTLI7AZ9LZDmHnAQwsi59Cc1Vd6Z%2BmZ5fvTALbBBPmfKLYnQ5lNDe35dlwbWSMIShDYX4YKLQOcw%2FQdRoEXG3RhikbYBqhSVo%2BVMrTfeSHmNZ0UYwtLvFUZlvWLdyGP2oVcBtQ3uJLcsd%2BBJyrtZXBtcOmY27ZGze0Q%2BtXRlM4OxtarJoVrbEtunAYIkKGowOqmvF72DMlPmeRLVevTCVcmCEhb%2B5%2BbgCLWD5ufmjwVaBxgrKyGzgTjgvZMIoXgNJhIjWUGDKY0vSeajBHbeykyaAhfbmRc6T9Q91MqoVII6pyQfJZp5Z5S6b8qS3ek8m%2Bo64ifB9DVeZ8ffla9GlFdp8QvtZweSeq%2F6JWB5PpePGbKsLtCLV4b63BT%2Bxnl2%2F4YnHIcETcJifOE8sb44IMxQMdLiAuv3bD%2B9mTbJCjcXRV9u63Jxc25fjJChoN4ZCG5Hv1T%2FoDPeAT2ZD%2BWCfnsQ%3D%3D&amp;nvMid=19298157033&amp;catId=50000153</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>LG전자 울트라HD 32UN650</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>548,880원</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>6,821개</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>https://cr.shopping.naver.com/adcr.nhn?x=cmsb2aWzBzMfXzbaTC%2FpWP%2F%2F%2Fw%3D%3DsmOt1z0n1WI%2FXO%2FTchJ5Qd7I26s45mHLBznrlDrP%2FYgRQ3qrx3p0MRIb3ekawSdvJUlCJOeLqKgaQQT2kIFznIjF58jfAIBSb%2BHVg6fYTWJTOBrkH5eL%2BGiYgkRcbqqAc3bHOcygeCu4ZWtd%2FrJCted9%2BKy%2Fm0d%2BgYWHtEf61Jo5CNclKwvLyA%2Fys%2F%2FHPPajL8qOEw8N3Ot5kqRKUpoGgeyKH4uGhdMZI%2BTAm7Oh3XZYWq6062OEPPa9WB%2BtWbtCGjgKe6djeuWuGZllC7f3Jz6sJF1TG8DXvuOXRWh2aiSE1QmeK3ZPITzKHcbEnR%2BI8wp0RCI5DZ%2BlLMCzrG1OOeEAg57IbU2vM5MZWiudNX5pXfqiCwBtPYYwEdSt6i2JAJiXHtSYHjGZPKmDvDzdKI4wrDmcefVedunKB1eUqYY3Id7fd%2Bwn%2FgkXeEKCjn4sGboyrgZ59kA7D8hqoEbuRvhwpWeMv%2FOn75GdIxWP%2F9t1sDgXhJyDhcIMVXp%2Fsg%2FEQT%2BDzDxwp7nT02YxkVA94lP3uR219qXNGACIy%2FSBaGSrynIE5iycn0Jeffj58JfYjnLywBF6TPdyrHi5pSyQkVg1QmAmnoJRdq4K9btjkCM0%3D&amp;nvMid=24635274522&amp;catId=50000153</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>LG전자 24MQ400</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>154,000원</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>364개</t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>https://cr.shopping.naver.com/adcr.nhn?x=ShEnb0CnlFYQnC6d8wjZa%2F%2F%2F%2Fw%3D%3Ds6QVyZMecK8JY4AMCQBsskV7of%2FCQYIKD2Rx9IN8sx13kEFD9EqEzeuo8lvy6ZeyvBM3rKhjjyZC5U51%2BQeC9eFUDpZsgzFAFORfT0UtaVWZ7h4YxfqVFkPRVarjF1EJTLI7AZ9LZDmHnAQwsi59Cc1Vd6Z%2BmZ5fvTALbBBPmfKLNdCsbapg1vrCtTKPdTR3C3GBrEFtGcbSlQTe8uXwC8SkbYBqhSVo%2BVMrTfeSHmNZ0UYwtLvFUZlvWLdyGP2oVcBtQ3uJLcsd%2BBJyrtZXBtcOmY27ZGze0Q%2BtXRlM4OxtarJoVrbEtunAYIkKGowOq%2Fvp3Us0sZNRp3GnWMfvO1yEhb%2B5%2BbgCLWD5ufmjwVaBxgrKyGzgTjgvZMIoXgNJhSDNcCyyriF1DB3euStHVTKAhfbmRc6T9Q91MqoVII6p60qpNSyMR62JHOt6I9TOWo64ifB9DVeZ8ffla9GlFdvEisOUBoyd6y9lBJ2vZssC%2FRhRXFpTt2%2FCbOS1hQrG%2BYnHIcETcJifOE8sb44IMxZB937iQtUmqlbcy6XcbCysDStNhbwnS4a%2B5zBhQtcyK5Hv1T%2FoDPeAT2ZD%2BWCfnsQ%3D%3D&amp;nvMid=36645806618&amp;catId=50000153</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>LG전자 32MN500MW</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>238,900원</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>6,634개</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>https://cr.shopping.naver.com/adcr.nhn?x=ctD3SkdDmFpr%2B1yGC41Vjf%2F%2F%2Fw%3D%3DsUy%2BocPhfeWMViJcH7tum%2FDUzP05u9G5KzpE279kHLvVQ3qrx3p0MRIb3ekawSdvJxuxiSI9xy0H1mQgZKX%2Bx6jF58jfAIBSb%2BHVg6fYTWJTOBrkH5eL%2BGiYgkRcbqqAc3bHOcygeCu4ZWtd%2FrJCted9%2BKy%2Fm0d%2BgYWHtEf61Jo5CNclKwvLyA%2Fys%2F%2FHPPajLED6qw1JBPa0EhRedL5KLaCKH4uGhdMZI%2BTAm7Oh3XZYWq6062OEPPa9WB%2BtWbtCGjgKe6djeuWuGZllC7f3Jz6sJF1TG8DXvuOXRWh2aiSE1QmeK3ZPITzKHcbEnR%2BI83lfZEFlMHk%2BKCcdlprJajSJFfssd8q%2FKljgM1C1p0VNXfqiCwBtPYYwEdSt6i2JA6xMz2an7mE6%2BKwxJoCwQN5iHcqLm1%2BFJXSTzsBvHXljId7fd%2Bwn%2FgkXeEKCjn4sGM%2BRAOjYlK%2BOXG8ZjY4xct8NQg3Yq6Ylx7b%2FrlGy3XKDyA95r585kcJGGKxpIuko6lMveu5pUmt5mX6mUy4ug6lgxRPGHGMebo4NuRbQz02E7LNIHLwWE4Usdio3mPK74sPdYG9o5dB2czTuk5ciFcx0cjwVm1BUYVknE7IEMpz4%3D&amp;nvMid=22764052560&amp;catId=50000153</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>벤큐 XL2411K</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>289,000원</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>2,859개</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>https://cr.shopping.naver.com/adcr.nhn?x=%2BHgcp03czgfKCnPtZmW4tf%2F%2F%2Fw%3D%3DsT9De3c4rX8XxvwkamLY18ppIhqVWM8hjP5C%2BZALTyGX6D9Doef8fQXU6eDjUh3hFrWR90H9ZDEWDKVxvYsW7KY4WQBe%2FZFkvs1gZ836hbpCe2umHfF2aLgG%2F437Vl%2B2i%2Br%2FdgAtqVYj6DoA7Mm4WZMv%2BjB2erv%2BZ%2Brrs5VHOiTQgGE7%2BZatKjf5hEf1XctkKkRJNtIMOsHYEPv9XvMd3epnNrwRClxwG6KI6Xy%2BWtBSkj8Xd80xPWZvn6URexO9BvdrxPgprIfciPgkJT4vsx0Pg%2F6PYJW9LpCSumzPJoigK7CtQzZWLlur1%2FFge4%2BEpPjGNpf6kA1v6Sb088A8WY46ASpVItOrM%2F6AL8l%2FuOwOkudW4LAgR4Xxl%2FdcF1QLKbX0gPuvaQnp9QR8ZlfHgWLL%2BD79JFqXUHChswIKAa5dTMw%2F8x3aoLIjogZLQtIW7g8p6%2FtaGyu3ul7LwRqGVwp2tomYFKYoY4Y0vhpHSm7EHr8NtjdOmZn5fiPIDRZn9nUpTzmQTeleeE0y%2Brv8xbBVWvDpk8rppPQr45vswK7cRqnWJlUEemzd2U3hiDA7uA35CyMrpXQUt3%2FJvHupy5s1ITc7NlRPvorKrNyQBKaY%3D&amp;nvMid=24196764522&amp;catId=50000153</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>벤큐 XL2546K</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>699,000원</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>1,003개</t>
-        </is>
-      </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>https://cr.shopping.naver.com/adcr.nhn?x=LFd5nsPLLl0YpDsv9YSXg%2F%2F%2F%2Fw%3D%3DsJi2yQLPAf1iAlK8%2BmvBI%2BbhOezuhHb1L0BZ1xIWyxW9Q3qrx3p0MRIb3ekawSdvJ2JliJGvMbiUoysUDTblD7TF58jfAIBSb%2BHVg6fYTWJTOBrkH5eL%2BGiYgkRcbqqAc3bHOcygeCu4ZWtd%2FrJCted9%2BKy%2Fm0d%2BgYWHtEf61Jo5CNclKwvLyA%2Fys%2F%2FHPPajL%2Fujts6GRjvv%2B8NnWJYGofCKH4uGhdMZI%2BTAm7Oh3XZYWq6062OEPPa9WB%2BtWbtCGjgKe6djeuWuGZllC7f3Jz6sJF1TG8DXvuOXRWh2aiSE1QmeK3ZPITzKHcbEnR%2BI8c7ZnDl0toOas4kDfZPtse5BC1CnJs1yZoWOj64R4bddXfqiCwBtPYYwEdSt6i2JAVTlSycrEagbLCXcRPxon5WJpKXtddjkok%2BQX32fGpjCXcIuRRvA%2Bz0rbBCGh3eLO1IMemlfv6iDotQSOeNmtb5lbzosDqu0bDzNqSLDi0aBNK36dfSxWxZLlaS%2F1zztKT%2BDzDxwp7nT02YxkVA94lJ9ALEbcpHHKSaYNNP%2F00jeMBau%2FXGWzdS5074%2BOZbd7Wsl5%2Bg4luaQ7gEP1gxuYzQ1QmAmnoJRdq4K9btjkCM0%3D&amp;nvMid=24235203522&amp;catId=50000153</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>한성컴퓨터 ULTRON 2760G 리얼</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>169,000원</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>8,103개</t>
-        </is>
-      </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>https://cr.shopping.naver.com/adcr.nhn?x=GbTt5%2FEak9ttNB3%2FsOLgr%2F%2F%2F%2Fw%3D%3DsjOprIZVK7HwV%2FbJ9Z1EDNWvJlg%2BwY8nX5DnzqELHcwv6D9Doef8fQXU6eDjUh3hFDSZH1RpNR%2Bb4xBl2eJJ%2B1Y4WQBe%2FZFkvs1gZ836hbpCe2umHfF2aLgG%2F437Vl%2B2i%2Br%2FdgAtqVYj6DoA7Mm4WZMv%2BjB2erv%2BZ%2Brrs5VHOiTQgGE7%2BZatKjf5hEf1XctkKDjrPGdhVkPsEQYZ0s2aLJpnNrwRClxwG6KI6Xy%2BWtBSkj8Xd80xPWZvn6URexO9BvdrxPgprIfciPgkJT4vsx0Pg%2F6PYJW9LpCSumzPJoigK7CtQzZWLlur1%2FFge4%2BEpjIGpOgUjfvfo4Rz7XsX4M5O%2FZHfw8y5T72RkNuXQ832kudW4LAgR4Xxl%2FdcF1QLKkR0Jufi%2B5Vfeao7xydTAm91woZLwre%2F0c6LfC8XQvOaPnD7hJV2J05mLBD5naU%2BlEw1kU3TPYVSgBvb0f8g%2FLfI0fIFRfBZUPaSLRPGc3PKufjygouZ%2BqG%2B1Tr8J%2BWq5e6MYUTPEr7lAfDH%2BW%2BhCTxGk4XMJtozo5T3u6g%2BJ%2BOvmKR3MMMkI56jGzHFDltYGAAAs8mMexu1dm2E8c5TJDscgIRCk8vtGb7Z%2FKGMSEdE%3D&amp;nvMid=15020041438&amp;catId=50000153</t>
+          <t>https://cr.shopping.naver.com/adcr.nhn?x=iCwiuL1I7vmPAM4%2Bk8bZbP%2F%2F%2Fw%3D%3DsGj68O3Ze0AQox90aPDZEUiQfgZwCAWeojltcUZSyPV76D9Doef8fQXU6eDjUh3hFLGbC1E4RSG7un7sSvbdHN990lYqjsgb%2Flwx642gSpssQKb3gny%2BhmcHehTHkI9Y9gm95oC2yEe6xrBnXD61GF8v%2BjB2erv%2BZ%2Brrs5VHOiTQgGE7%2BZatKjf5hEf1XctkK9qSKXgoi8oGbG2WVp3jxEpnNrwRClxwG6KI6Xy%2BWtBSkj8Xd80xPWZvn6URexO9BvdrxPgprIfciPgkJT4vsx0Pg%2F6PYJW9LpCSumzPJoigK7CtQzZWLlur1%2FFge4%2BEpOtYnB4oADGX9J9Voxhe4pX%2FWznVghrW7V1QAaTE3E%2FqkudW4LAgR4Xxl%2FdcF1QLKWVzqUgdvCXmKg0W8CnHjKXzEWKIeSL8gCGko0muIXASpsBVMxBwX6oIWWdxUIiiXpqJykqIyDolEoVJ%2FMTE6pHIEOMyyDocZ9XLqN14mUSyjriJ8H0NV5nx9%2BVr0aUV2TsG9V1%2FA7%2FvBFoby9LtaxAd5tuM5ZrevXvYAbtXnelFicchwRNwmJ84TyxvjggzF%2Bs8iZixIWRLFY%2FAfUHJJEXFdVpY6uNSJ1AJpBNoNx7fke%2FVP%2BgM94BPZkP5YJ%2Bex&amp;nvMid=18778755031&amp;catId=50000153</t>
         </is>
       </c>
     </row>

</xml_diff>